<commit_message>
Remove gebruikersdoel from spreadsheets as this field's value is automatically added
</commit_message>
<xml_diff>
--- a/files/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/files/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="1103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="1099">
   <si>
     <t>Toelichting</t>
   </si>
@@ -3116,20 +3116,6 @@
     <t>Stadhuis</t>
   </si>
   <si>
-    <t>Gebruikersdoel het gebouw</t>
-  </si>
-  <si>
-    <t>Gebruiksdoel volgens de BAG.
-Voor uitgebreidere beschrijving van bovenstaande gebruiksdoelen zie: https://www.amsterdam.nl/stelselpedia/bag-index/handboek-inwinnen/introductie-bag/registratie/gebruiksdoel/
-Gebruiksdoel van elk gebouw is te vinden door het adres op https://bagviewer.kadaster.nl/ in te voeren en rechts onder het kopje 'Verblijfsobject' te kijken.</t>
-  </si>
-  <si>
-    <t>keuze uit: 'Wonen', 'Bijeenkomst', 'Winkel', 'Gezondheidszorg', 'Kantoor', 'Logies', 'Industrie', 'Onderwijs', 'Sport', 'Overig', 'Cel'</t>
-  </si>
-  <si>
-    <t>Kantoor</t>
-  </si>
-  <si>
     <t>Website locatie</t>
   </si>
   <si>
@@ -3398,7 +3384,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3485,11 +3471,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3582,11 +3563,11 @@
     <xf numFmtId="164" fontId="11" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3699,10 +3680,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3751,11 +3728,11 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="22" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="23" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="24" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3897,7 +3874,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:ALQ17"/>
+  <dimension ref="A1:ALQ16"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -6993,21 +6970,21 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>1017</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1011</v>
+        <v>1018</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>1018</v>
-      </c>
-      <c r="D4" s="15" t="s">
         <v>1019</v>
       </c>
+      <c r="D4" s="11" t="s">
+        <v>1020</v>
+      </c>
       <c r="E4" s="16" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="14"/>
@@ -7023,25 +7000,25 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>1022</v>
+        <v>1011</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>1023</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="15" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>1024</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>1025</v>
-      </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
@@ -7053,25 +7030,21 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>1026</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>1027</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>1013</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>1028</v>
-      </c>
-      <c r="F6" s="17"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="18"/>
+      <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -7083,19 +7056,23 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>1029</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="E7" s="13" t="n">
+        <v>4.3166395</v>
+      </c>
+      <c r="F7" s="13"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -7111,19 +7088,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>1011</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="E8" s="13" t="n">
-        <v>4.3166395</v>
+        <v>52.0775912</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="14"/>
@@ -7141,20 +7118,14 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>1033</v>
-      </c>
-      <c r="E9" s="13" t="n">
-        <v>52.0775912</v>
-      </c>
+        <v>1018</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -7169,17 +7140,23 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>1036</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -7193,25 +7170,25 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
         <v>1037</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>1011</v>
+        <v>1018</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>1038</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="11" t="s">
         <v>1039</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>1040</v>
-      </c>
-      <c r="F11" s="19"/>
+      <c r="E11" s="16" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F11" s="16"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="H11" s="18"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -7223,25 +7200,23 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>1042</v>
-      </c>
+        <v>1018</v>
+      </c>
+      <c r="C12" s="20"/>
       <c r="D12" s="11" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>1011</v>
+        <v>1018</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="18"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
@@ -7255,17 +7230,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C13" s="20"/>
+        <v>1018</v>
+      </c>
+      <c r="C13" s="15"/>
       <c r="D13" s="11" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="14"/>
@@ -7283,17 +7258,17 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="11" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>1022</v>
+        <v>1011</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="14"/>
@@ -7309,35 +7284,35 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="21" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>1046</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="11" t="s">
-        <v>1043</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>1011</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
     </row>
-    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21" t="s">
         <v>1047</v>
       </c>
@@ -7348,10 +7323,10 @@
         <v>1048</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>1049</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>1050</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -7364,34 +7339,6 @@
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
-    </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="s">
-        <v>1051</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>1052</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>1024</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>1053</v>
-      </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7441,7 +7388,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
@@ -7459,19 +7406,19 @@
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>1011</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>1057</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>1058</v>
+        <v>1053</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>1054</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -7489,19 +7436,19 @@
     </row>
     <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1060</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>1061</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>1058</v>
+        <v>1056</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>1054</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="14"/>
@@ -7518,20 +7465,20 @@
       <c r="R3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="s">
-        <v>1062</v>
+      <c r="A4" s="29" t="s">
+        <v>1058</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>1011</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>1058</v>
+        <v>1060</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>1054</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -7548,20 +7495,20 @@
       <c r="R4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
-        <v>1065</v>
-      </c>
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="29" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>1011</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="31" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>1015</v>
       </c>
-      <c r="E5" s="33" t="s">
-        <v>1067</v>
+      <c r="E5" s="32" t="s">
+        <v>1063</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="14"/>
@@ -7578,20 +7525,20 @@
       <c r="R5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
-        <v>1068</v>
-      </c>
-      <c r="B6" s="31" t="s">
+      <c r="A6" s="29" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B6" s="30" t="s">
         <v>1011</v>
       </c>
-      <c r="C6" s="32" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D6" s="34" t="s">
+      <c r="C6" s="31" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>1015</v>
       </c>
-      <c r="E6" s="34" t="s">
-        <v>1069</v>
+      <c r="E6" s="33" t="s">
+        <v>1065</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -7608,20 +7555,20 @@
       <c r="R6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C7" s="32" t="s">
+      <c r="A7" s="29" t="s">
         <v>1066</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="B7" s="30" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>1015</v>
       </c>
-      <c r="E7" s="34" t="s">
-        <v>1071</v>
+      <c r="E7" s="33" t="s">
+        <v>1067</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -7638,20 +7585,20 @@
       <c r="R7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="s">
-        <v>1072</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D8" s="34" t="s">
+      <c r="A8" s="29" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>1015</v>
       </c>
-      <c r="E8" s="34" t="s">
-        <v>1073</v>
+      <c r="E8" s="33" t="s">
+        <v>1069</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -7668,20 +7615,20 @@
       <c r="R8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
-        <v>1074</v>
+      <c r="A9" s="29" t="s">
+        <v>1070</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>1058</v>
+        <v>1072</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>1054</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="14"/>
@@ -7698,18 +7645,18 @@
       <c r="R9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="s">
-        <v>1077</v>
-      </c>
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="29" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>1011</v>
       </c>
-      <c r="C10" s="32" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34" t="s">
-        <v>1078</v>
+      <c r="C10" s="31" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33" t="s">
+        <v>1074</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -7726,18 +7673,18 @@
       <c r="R10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30" t="s">
-        <v>1079</v>
-      </c>
-      <c r="B11" s="31" t="s">
+      <c r="A11" s="29" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>1011</v>
       </c>
-      <c r="C11" s="32" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34" t="s">
-        <v>1080</v>
+      <c r="C11" s="31" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33" t="s">
+        <v>1076</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="14"/>
@@ -7754,20 +7701,20 @@
       <c r="R11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
-        <v>1081</v>
+      <c r="A12" s="29" t="s">
+        <v>1077</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>1058</v>
+        <v>1079</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>1054</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="14"/>
@@ -7784,18 +7731,18 @@
       <c r="R12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="s">
-        <v>1084</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35" t="s">
-        <v>1085</v>
+      <c r="A13" s="29" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34" t="s">
+        <v>1081</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="1"/>
@@ -7812,24 +7759,24 @@
       <c r="R13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
-        <v>1086</v>
+      <c r="A14" s="29" t="s">
+        <v>1082</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>1088</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>1089</v>
+        <v>1084</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>1085</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="37"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="14"/>
       <c r="J14" s="1"/>
       <c r="K14" s="14"/>
@@ -7842,24 +7789,24 @@
       <c r="R14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="s">
-        <v>1090</v>
+      <c r="A15" s="29" t="s">
+        <v>1086</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>1011</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>1091</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>1093</v>
+        <v>1087</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>1089</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="37"/>
+      <c r="H15" s="36"/>
       <c r="I15" s="14"/>
       <c r="J15" s="1"/>
       <c r="K15" s="14"/>
@@ -7872,22 +7819,22 @@
       <c r="R15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="s">
-        <v>1094</v>
-      </c>
-      <c r="B16" s="31" t="s">
+      <c r="A16" s="29" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B16" s="30" t="s">
         <v>1011</v>
       </c>
-      <c r="C16" s="32" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38" t="s">
-        <v>1095</v>
+      <c r="C16" s="31" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37" t="s">
+        <v>1091</v>
       </c>
       <c r="F16" s="27"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="37"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="14"/>
       <c r="J16" s="1"/>
       <c r="K16" s="14"/>
@@ -7900,18 +7847,18 @@
       <c r="R16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>1097</v>
-      </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="33" t="s">
-        <v>1098</v>
+      <c r="A17" s="29" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="32" t="s">
+        <v>1094</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="1"/>
@@ -7928,20 +7875,20 @@
       <c r="R17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30" t="s">
-        <v>1099</v>
+      <c r="A18" s="29" t="s">
+        <v>1095</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>

</xml_diff>

<commit_message>
Freeze the first row and first two columns
</commit_message>
<xml_diff>
--- a/files/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/files/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -4419,9 +4419,11 @@
   <dimension ref="A1:ALQ95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9270,7 +9272,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="21.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="80.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="85.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="23" width="74.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="23" width="11.52"/>

</xml_diff>

<commit_message>
Implement Stembureaus ODS v1.3 changes; small fixes with removal of afgiftepunten
</commit_message>
<xml_diff>
--- a/files/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/files/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -22,24 +22,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="1134">
   <si>
     <t xml:space="preserve">Toelichting</t>
   </si>
   <si>
     <t xml:space="preserve">Op dit tabblad wordt het gebruik van deze spreadsheet toegelicht. Hieronder staat de beschrijving van de andere twee tabbladen 'Attributen' en 'Metadata'.
 Dit invulformulier is bedoeld om geüpload te worden naar https://waarismijnstemlokaal.nl/. In plaats van dit invulformulier kan ook de invultool op https://waarismijnstemlokaal.nl/ gebruikt worden. Ook kan op die website een versie van dit invulformulier gedownload worden waarin de stembureaus van de vorige verkiezing alvast (deels) ingevuld staan.
-Dit invulformulier is gebaseerd op de Stembureaus Open Data Standaard versie 1.2.</t>
+Dit invulformulier is gebaseerd op de Stembureaus Open Data Standaard versie 1.3.</t>
   </si>
   <si>
     <t xml:space="preserve">Attributen</t>
   </si>
   <si>
-    <t xml:space="preserve">Op het tabblad 'Attributen' kunt u alle stembureaus/afgiftepunten in uw gemeente toevoegen.
-Elk stembureau/afgiftepunt voegt u toe in een eigen 'Invulveld'-kolom waar u minimaal alle verplichte attributen (aangegeven met 'Y') invult (NB: in sommige gevallen kan hiervan worden afgeweken zoals beschreven in de opmerkingen bij een attribuut).
+    <t xml:space="preserve">Op het tabblad 'Attributen' kunt u alle stembureaus in uw gemeente toevoegen.
+Elk stembureau voegt u toe in een eigen 'Invulveld'-kolom waar u minimaal alle verplichte attributen (aangegeven met 'ja') invult (NB: in sommige gevallen kan hiervan worden afgeweken zoals beschreven in de opmerkingen bij een attribuut).
 De kolommen 'Opmerkingen, 'Format' en 'Voorbeeld' helpen u daarbij. De 'Opmerkingen'-kolom geeft algemene informatie over het attribuut en geeft soms meer informatie over hoe u het veld moet invullen zoals gespecificeerd in de 'Format'-kolom. In de 'Voorbeeld'-kolom wordt een voorbeeld gegeven van hoe u het attribuut moet invullen.
 Sommige gemeenten werken met mobiele stembureaus die gedurende de dag op verschillende locaties staan. Voor mobiele stembureaus moet elke locatie apart worden ingevoerd in een eigen 'Invulveld'-kolom (vul dus hele kolom in en niet enkel de attributen die veranderen, zoals de locatie en openingstijden).
-Er zijn 1000 'Invulveld'-kolommen, aangezien de gemeente met de meeste stembureaus (Amsterdam) er bijna 500 heeft en er voor mobiele stembureaus dus meerdere 'Invulveld'-kolommen nodig zijn. Daarbovenop komen nog de afgiftepunten die nu ook verzameld worden. Mocht dit toch niet genoeg zijn dan kunt u gewoon extra kolommen aanmaken en ze doornummeren.</t>
+Er zijn 1000 'Invulveld'-kolommen, aangezien de gemeente met de meeste stembureaus (Amsterdam) er bijna 500 heeft en er voor mobiele stembureaus dus meerdere 'Invulveld'-kolommen nodig zijn. Mocht dit toch niet genoeg zijn dan kunt u gewoon extra kolommen aanmaken en ze doornummeren.</t>
   </si>
   <si>
     <t xml:space="preserve">Metadata</t>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">Dit tabblad bevat de metadata van deze dataset. Alle velden zijn al ingevuld en puur ter informatie. Ze hoeven dus niet door u aangepast te worden. Voor de metadata wordt gebruik gemaakt van de DCAT standaard: https://data.overheid.nl/dcat. Velden die elke verkiezing hetzelfde blijven hebben ter verduidelijking een grijze achtergrond gekregen.</t>
   </si>
   <si>
-    <t xml:space="preserve">Verplicht (Y/N)</t>
+    <t xml:space="preserve">Verplicht (ja/nee)</t>
   </si>
   <si>
     <t xml:space="preserve">Opmerkingen</t>
@@ -3060,229 +3060,150 @@
     <t xml:space="preserve">Invulveld 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Stembureau of Afgiftepunt</t>
+    <t xml:space="preserve">Nummer stembureau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Een stembureau is gevestigd in een stemlokaal en elk stembureau heeft een eigen nummer. Sommige stemlokalen hebben meerdere stembureaus. Elk stembureau moet apart ingevoerd ook al is de locatie (het stemlokaal) hetzelfde aangezien elk stembureau een ander nummer heeft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cijfers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naam stembureau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stadhuis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website van de locatie van het stembureau, indien aanwezig; Een URL moet met 'http://' of 'https://' beginnen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.denhaag.nl/nl/bestuur-en-organisatie/contact-met-de-gemeente/stadhuis-den-haag.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG Nummeraanduiding ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG Nummeraanduiding ID, vindbaar door het adres van het stembureau op https://bagviewer.kadaster.nl/ in te voeren en rechts onder het kopje 'Nummeraanduiding' te kijken.
+Vermeld voor mobiele stembureaus of locaties zonder BAG Nummeraanduiding ID het dichtstbijzijnde BAG Nummeraanduiding ID en gebruik eventueel het 'Extra adresaanduiding'-veld om de locatie van stembureau te beschrijven. NB: de precieze locatie geeft u aan met de 'Latitude' en 'Longitude'-velden of met de ‘X’ en ‘Y’-velden.
+Caribisch Nederland (BES-eilanden) staat niet in de BAG. Deze gemeenten moeten '0000000000000000' (zestien keer het getal '0') invullen en het adres verplicht invullen in het 'Extra adresaanduiding'-attribuut.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0518200000747446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra adresaanduiding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja, als er '0000000000000000' is ingevuld bij 'BAG Nummeraanduiding ID'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventuele extra informatie over de locatie van het stembureau. Bv. 'Ingang aan achterkant gebouw' of 'Mobiel stembureau op het midden van het plein'.
+Caribisch Nederland (BES-eilanden) vult verplicht hier het hele adres in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingang aan achterkant gebouw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja, alleen als er geen 'BAG Nummeraanduiding ID' beschikbaar is of er een 'BAG Nummeraanduiding ID' gekozen is dat niet precies het adres/de locatie van het stembureau betreft.
+Dan moet er Latitude én Longitude of X én Y ingevuld zijn. (Als alle vier de velden zijn ingevuld dan worden de waarden van Longitude en Latitude gebruikt om X en Y te berekenen als er een verschil is tussen de coördinaten).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rijksdriehoekscoördinaat x (minimaal in meters, decimalen ook toegestaan).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getal tussen 0 en 300000</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Voor de Tweede Kamerverkiezingen van 2021 zijn er vanwege de maatregelen rondom het coronavirus naast stembureaus ook afgiftepunten beschikbaar. Iedereen ouder dan 70 ontvangt een stempluspas die op de post gedaan kan worden maar ook in de dagen voor en op de verkiezingsdag ingeleverd kan worden bij een afgiftepunt. Via deze standaard wordt zowel informatie over stembureaus als afgiftepunten verzameld.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keuze uit: ‘Stembureau’, ‘Afgiftepunt’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afgiftepunt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nummer stembureau of afgiftepunt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Een stembureau is gevestigd in een stemlokaal en elk stembureau heeft een eigen nummer. Sommige stemlokalen hebben meerdere stembureaus. Elk stembureau moet apart ingevoerd ook al is de locatie (het stemlokaal) hetzelfde aangezien elk stembureau een ander nummer heeft.
-Dit attribuut is niet verplicht voor afgiftepunten.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cijfers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naam stembureau of afgiftepunt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dit attribuut is niet verplicht voor afgiftepunten.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tekst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stadhuis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website van de locatie van het stembureau/afgiftepunt, indien aanwezig; Een URL moet met 'http://' of 'https://' beginnen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.denhaag.nl/nl/bestuur-en-organisatie/contact-met-de-gemeente/stadhuis-den-haag.htm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG referentie nummer</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BAG Nummeraanduiding ID, vindbaar door het adres van het stembureau/afgiftepunt op https://bagviewer.kadaster.nl/ in te voeren en rechts onder het kopje 'Nummeraanduiding' te kijken.
-Vermeld voor mobiele stembureaus of lokaties zonder BAG Nummeraanduiding ID het dichtstbijzijnde BAG Nummeraanduiding ID en gebruik eventueel het 'Extra adresaanduiding'-veld om de locatie van stembureau te beschrijven. NB: de precieze locatie geeft u aan met de 'Latitude' en 'Longitude'-velden </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">of met de ‘X’ en ‘Y’-velden.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-Caribisch Nederland (BES-eilanden) staat niet in de BAG. Deze gemeenten moeten “0000000000000000” (zestien keer het getal "0") invullen en het adres verplicht invullen in het ‘Extra adresaanduiding’-attribuut.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">0518200000747446</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extra adresaanduiding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eventuele extra informatie over de locatie van het stembureau/afgiftepunt. Bv. 'Ingang aan achterkant gebouw' of 'Mobiel stembureau op het midden van het plein'.
-Caribisch Nederland (BES-eilanden) vult verplicht hier het hele adres in.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingang aan achterkant gebouw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimaal Longitude én Latitude of X én Y moeten ingevuld zijn. (Als alle vier de velden zijn ingevuld dan worden de waarden van Longitude en Latitude gebruikt om X en Y te berekenen als er een verschil is tussen de coördinaten).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rijksdriehoekscoördinaat x (minimaal in meters, decimalen ook toegestaan).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">getal tussen 0 en 300000</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rijksdriehoekscoördinaat y (minimaal in meters, decimalen ook toegestaan).</t>
   </si>
   <si>
     <t xml:space="preserve">getal tussen 300000 en 620000</t>
   </si>
   <si>
+    <t xml:space="preserve">Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breedtegraad (DD.dddddd notatie), bv. 52.0775912; minimaal 4 decimalen.
+Als u de latitude van het stembureau niet weet dan kunt u dit vinden via https://www.openstreetmap.org/. Zoom in op het stembureau, klik op de juiste locatie met de rechtermuisknop en selecteer 'Show address'/'Toon adres'. De latitude en longitude (in die volgorde) staan nu linksboven in de zoekbalk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graden in DD.dddddd notatie; minimaal 4 decimalen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Longitude</t>
   </si>
   <si>
     <t xml:space="preserve">Lengtegraad (DD.dddddd notatie), bv. 4.3166395; minimaal 4 decimalen.
-Als u de longitude van het stembureau/afgiftepunt niet weet dan kunt u dit vinden via https://www.openstreetmap.org/. Zoom in op het stembureau/afgiftepunt, klik op de juiste locatie met de rechtermuisknop en selecteer "Show address"/"Toon adres". De latitude en longitude (in die volgorde) staan nu linksboven in de zoekbalk.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">graden in DD.dddddd notatie; minimaal 4 decimalen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breedtegraad (DD.dddddd notatie), bv. 52.0775912; minimaal 4 decimalen.
-Als u de latitude van het stembureau/afgiftepunt niet weet dan kunt u dit vinden via https://www.openstreetmap.org/. Zoom in op het stembureau/afgiftepunt, klik op de juiste locatie met de rechtermuisknop en selecteer "Show address"/"Toon adres". De latitude en longitude (in die volgorde) staan nu linksboven in de zoekbalk.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 10-03-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voor een afgiftepunt moet er minimaal 1 openingstijden-attribuut ingevuld worden.
-Dit attribuut is niet verplicht voor stembureaus aangezien die enkel op 15-17 maart open zijn.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sommige gemeenten werken met mobiele stembureaus die gedurende de dag op verschillende locaties staan. Voor mobiele stembureaus moet elke locatie apart worden ingevoerd in een eigen 'Invulveld'-kolom (vul dus de hele kolom in en niet enkel de attributen die veranderen, zoals de locatie en openingstijden).
-Tijdens de Tweede Kamerverkiezingen van 2021 wordt er op meerdere dagen gestemd via zowel stembureaus (3 dagen) als afgiftepunten (8 dagen).</t>
+Als u de longitude van het stembureau niet weet dan kunt u dit vinden via https://www.openstreetmap.org/. Zoom in op het stembureau, klik op de juiste locatie met de rechtermuisknop en selecteer 'Show address'/'Toon adres". De latitude en longitude (in die volgorde) staan nu linksboven in de zoekbalk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Openingstijden 14-03-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja, voor een stembureau moet er minimaal 1 openingstijden-attribuut ingevuld worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zie opmerking bij het ‘Openingstijden 16-03-2022’-attribuut</t>
   </si>
   <si>
     <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS tot YYYY-MM-DDTHH:MM:SS</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-03-10T07:30:00 tot 2021-03-10T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 11-03-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zie beschrijving bij het ‘Openingstijden 10-03-2021’-attribuut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zie opmerking bij het ‘Openingstijden 10-03-2021’-attribuut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-03-11T07:30:00 tot 2021-03-11T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 12-03-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-03-12T07:30:00 tot 2021-03-12T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 13-03-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-03-13T07:30:00 tot 2021-03-13T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 14-03-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-03-14T07:30:00 tot 2021-03-14T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 15-03-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voor een stembureau of afgiftepunt moet er minimaal 1 openingstijden-attribuut ingevuld worden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-03-15T07:30:00 tot 2021-03-15T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 16-03-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zie beschrijving bij het ‘Openingstijden 15-03-2021’-attribuut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-03-16T07:30:00 tot 2021-03-16T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 17-03-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021-03-17T07:30:00 tot 2021-03-17T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mindervaliden toegankelijk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is het stembureau/afgiftepunt toegankelijk voor mindervaliden?
+    <t xml:space="preserve">2022-03-14T07:30:00 tot 2022-03-14T21:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Openingstijden 15-03-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-15T07:30:00 tot 2022-03-15T21:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Openingstijden 16-03-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sommige gemeenten werken met mobiele stembureaus die gedurende de dag op verschillende locaties staan. Voor mobiele stembureaus moet elke locatie apart worden ingevoerd in een eigen 'Invulveld'-kolom (vul dus de hele kolom in en niet enkel de attributen die veranderen, zoals de locatie en openingstijden).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-16T07:30:00 tot 2022-03-16T21:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toegankelijk voor mensen met een lichamelijke beperking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is het stembureau toegankelijk voor mensen met een lichamelijke beperking?
 Voor meer informatie, zie:
-https://www.rijksoverheid.nl/documenten/publicaties/2018/10/25/toolkit-verkiezingen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y of N</t>
+https://www.rijksoverheid.nl/documenten/publicaties/2021/10/14/toegankelijkheid-verkiezingen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja of nee</t>
   </si>
   <si>
     <t xml:space="preserve">Akoestiek</t>
   </si>
   <si>
-    <t xml:space="preserve">Is de akoestiek van het stembureau/afgiftepunt geschikt voor slechthorenden?
+    <t xml:space="preserve">Is de akoestiek van het stembureau geschikt voor slechthorenden?
 Voor meer informatie, zie: https://bk.nijsnet.com/04040_Slechthorenden.aspx</t>
   </si>
   <si>
@@ -3292,7 +3213,7 @@
     <t xml:space="preserve">Welke auditieve hulpmiddelen zijn aanwezig? Dit is een vrij tekstveld.</t>
   </si>
   <si>
-    <t xml:space="preserve">Doventolk, ringleiding</t>
+    <t xml:space="preserve">gebarentolk</t>
   </si>
   <si>
     <t xml:space="preserve">Visuele hulpmiddelen</t>
@@ -3301,13 +3222,13 @@
     <t xml:space="preserve">Welke visuele hulpmiddelen zijn aanwezig? Dit is een vrij tekstveld.</t>
   </si>
   <si>
-    <t xml:space="preserve">Leesloep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mindervalide toilet aanwezig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is er een mindervalide toilet aanwezig? </t>
+    <t xml:space="preserve">leesloep, stemmal, vrijwilliger/host aanwezig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gehandicaptentoilet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is er een gehandicaptentoilet aanwezig? </t>
   </si>
   <si>
     <t xml:space="preserve">Tellocatie</t>
@@ -3316,10 +3237,10 @@
     <t xml:space="preserve">Is deze locatie ook een locatie waar de stemmen worden geteld?</t>
   </si>
   <si>
-    <t xml:space="preserve">Contactgegevens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;afdeling/functie&gt;: De afdeling of specifieke functie binnen de gemeente die zich bezig houdt met de stembureaus/afgiftepunten; ivm verduurzaming bij voorkeur dus niet de naam/contactgegevens van een persoon</t>
+    <t xml:space="preserve">Contactgegevens gemeente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;afdeling/functie&gt;: De afdeling of specifieke functie binnen de gemeente die zich bezig houdt met de stembureaus; ivm verduurzaming bij voorkeur dus niet de naam/contactgegevens van een persoon.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;afdeling/functie&gt;, &lt;e-mailadres en/of telefoonnummer en/of postadres&gt;</t>
@@ -3328,16 +3249,13 @@
     <t xml:space="preserve">Unit Verkiezingen, verkiezingen@denhaag.nl 070-3534488 Gemeente Den Haag Publiekszaken/Unit Verkiezingen Postbus 84008 2508 AA Den Haag</t>
   </si>
   <si>
-    <t xml:space="preserve">Beschikbaarheid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URL van de gemeentewebsite met data of informatie over de stembureaus/afgiftepunten (of verkiezingen); Een URL moet met 'http://' of 'https://' beginnen.</t>
+    <t xml:space="preserve">Verkiezingswebsite gemeente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL van de gemeentewebsite met data of informatie over de stembureaus (of verkiezingen); Een URL moet met 'http://' of 'https://' beginnen.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.stembureausindenhaag.nl/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invulveld</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
@@ -3350,13 +3268,13 @@
     <t xml:space="preserve">Stembureaus &lt;verkiezing&gt; &lt;jaar&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;wordt automatisch ingevuld afhankelijk van de verkiezing&gt;</t>
+    <t xml:space="preserve">Stembureaus gemeenteraadsverkiezingen 2022</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;CBS gemeentecode&gt;: code bestaande uit 6 karakters, zie https://opendata.cbs.nl/#/CBS/nl/dataset/84929NED/table?dl=B165
+    <t xml:space="preserve">&lt;CBS gemeentecode&gt;: code bestaande uit 6 karakters, zie https://opendata.cbs.nl/statline/#/CBS/nl/dataset/85067NED/table?dl=B165 of gebruik GM9001 voor Bonaire, GM9002 voor Sint Eustatius of GM9003 voor Saba.
 &lt;YYYYMMDD&gt;: datum van de verkiezing
 &lt;oplopend getal&gt;: getal tussen 000 en 999</t>
   </si>
@@ -3364,14 +3282,20 @@
     <t xml:space="preserve">NLODS&lt;CBS gemeentecode&gt;stembureaus&lt;YYYYMMDD&gt;&lt;oplopend getal van 000 t/m 999&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">NLODSGM0518stembureaus20220316009</t>
+  </si>
+  <si>
     <t xml:space="preserve">Omschrijving</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;verkiezing&gt;: keuze uit 'de Tweede Kamerverkiezingen', 'de gemeenteraadsverkiezingen', 'de Provinciale Statenverkiezingen', 'referendum &lt;naam van referendum&gt;', 'de kiescollegeverkiezingen', 'de eilandsraadsverkiezingen', 'de Europees Parlementsverkiezingen', 'de waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'
-&lt;datum&gt;: in format zoals '17 maart 2021'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overzicht van de locaties van stembureaus en afgiftepunten. De gegevens hebben betrekking op &lt;verkiezing&gt; op &lt;datum&gt;.</t>
+&lt;datum&gt;: in format zoals '16 maart 2022'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op &lt;verkiezing&gt; op &lt;datum&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op de gemeenteraadsverkiezingen op 16 maart 2022.</t>
   </si>
   <si>
     <t xml:space="preserve">Eigenaar</t>
@@ -3407,7 +3331,10 @@
     <t xml:space="preserve">&lt;aard van de verkiezing&gt;: keuze uit 'Tweede Kamerverkiezingen', 'gemeenteraadsverkiezingen', 'Provinciale Statenverkiezingen', 'referendum', 'eilandsraadsverkiezingen', 'kiescollegeverkiezingen', 'Europees Parlementsverkiezingen', 'waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'</t>
   </si>
   <si>
-    <t xml:space="preserve">verkiezingen, stembureaus, afgiftepunten, overheid, democratie, stemmen, kiesdistrict, &lt;aard van de verkiezing&gt;</t>
+    <t xml:space="preserve">verkiezingen, stembureaus, overheid, democratie, stemmen, kiesdistrict, &lt;aard van de verkiezing&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verkiezingen, stembureaus, overheid, democratie, stemmen, kiesdistrict, gemeenteraadsverkiezingen</t>
   </si>
   <si>
     <t xml:space="preserve">Thema</t>
@@ -3436,6 +3363,9 @@
     <t xml:space="preserve">&lt;gebied&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">Europees Nederland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Datum publicatie</t>
   </si>
   <si>
@@ -3445,6 +3375,9 @@
     <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS+-HH:MM</t>
   </si>
   <si>
+    <t xml:space="preserve">2022-01-16T13:05:23+01:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Relatie / gebruik andere standaarden</t>
   </si>
   <si>
@@ -3460,16 +3393,19 @@
     <t xml:space="preserve">YYYY-MM-DD</t>
   </si>
   <si>
+    <t xml:space="preserve">2022-03-16</t>
+  </si>
+  <si>
     <t xml:space="preserve">Update frequentie</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;datum verkiezing&gt;: in format zoals '17 maart 2021'</t>
+    <t xml:space="preserve">&lt;datum verkiezing&gt;: in format zoals '16 maart 2022'</t>
   </si>
   <si>
     <t xml:space="preserve">Incidenteel tot en met &lt;datum verkiezing&gt; (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezing)</t>
   </si>
   <si>
-    <t xml:space="preserve">Incidenteel tot en met 17 maart 2021 (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezingen)</t>
+    <t xml:space="preserve">Incidenteel tot en met 16 maart 2022 (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezingen)</t>
   </si>
   <si>
     <t xml:space="preserve">Wijzigings datum</t>
@@ -3491,7 +3427,7 @@
 Invoer is "vast"</t>
   </si>
   <si>
-    <t xml:space="preserve">Stembureaus ODS 1.2</t>
+    <t xml:space="preserve">Stembureaus ODS 1.3</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -3505,6 +3441,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;status&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In ontwikkeling</t>
   </si>
   <si>
     <t xml:space="preserve">Beschikbare formaten</t>
@@ -3525,7 +3464,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3677,14 +3616,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -3701,21 +3632,23 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -3785,14 +3718,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -3826,7 +3759,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3850,57 +3783,99 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
@@ -3913,32 +3888,38 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3963,20 +3944,24 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="42" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="42" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="60" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3987,63 +3972,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="44" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="61" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="45" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="46" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="46" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="47" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="46" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="46" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="48" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4055,16 +4032,28 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -4075,15 +4064,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4095,7 +4084,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="42" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4103,28 +4092,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="46" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="48" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="47" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="48" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="46" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="46" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -4132,7 +4121,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="51">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -4140,34 +4129,50 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Accent 1 18" xfId="21"/>
-    <cellStyle name="Accent 17" xfId="22"/>
-    <cellStyle name="Accent 2 19" xfId="23"/>
-    <cellStyle name="Accent 3 20" xfId="24"/>
-    <cellStyle name="Bad 14" xfId="25"/>
-    <cellStyle name="Error 16" xfId="26"/>
-    <cellStyle name="Footnote 9" xfId="27"/>
-    <cellStyle name="Good 12" xfId="28"/>
-    <cellStyle name="Heading 1 5" xfId="29"/>
-    <cellStyle name="Heading 2 6" xfId="30"/>
-    <cellStyle name="Heading 3" xfId="31"/>
-    <cellStyle name="Heading 4" xfId="32"/>
-    <cellStyle name="Heading1" xfId="33"/>
-    <cellStyle name="Hyperlink 10" xfId="34"/>
-    <cellStyle name="Neutral 13" xfId="35"/>
-    <cellStyle name="Note 8" xfId="36"/>
-    <cellStyle name="Result" xfId="37"/>
-    <cellStyle name="Result2" xfId="38"/>
-    <cellStyle name="Status 11" xfId="39"/>
-    <cellStyle name="Text 7" xfId="40"/>
-    <cellStyle name="Warning 15" xfId="41"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="42"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="43"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="44"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="45"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="46"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="47"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="48"/>
+    <cellStyle name="Accent 1 19" xfId="22"/>
+    <cellStyle name="Accent 17" xfId="23"/>
+    <cellStyle name="Accent 18" xfId="24"/>
+    <cellStyle name="Accent 2 19" xfId="25"/>
+    <cellStyle name="Accent 2 20" xfId="26"/>
+    <cellStyle name="Accent 3 20" xfId="27"/>
+    <cellStyle name="Accent 3 21" xfId="28"/>
+    <cellStyle name="Bad 14" xfId="29"/>
+    <cellStyle name="Bad 15" xfId="30"/>
+    <cellStyle name="Error 16" xfId="31"/>
+    <cellStyle name="Error 17" xfId="32"/>
+    <cellStyle name="Footnote 10" xfId="33"/>
+    <cellStyle name="Footnote 9" xfId="34"/>
+    <cellStyle name="Good 12" xfId="35"/>
+    <cellStyle name="Good 13" xfId="36"/>
+    <cellStyle name="Heading 1 5" xfId="37"/>
+    <cellStyle name="Heading 1 6" xfId="38"/>
+    <cellStyle name="Heading 2 6" xfId="39"/>
+    <cellStyle name="Heading 2 7" xfId="40"/>
+    <cellStyle name="Heading 3" xfId="41"/>
+    <cellStyle name="Heading 4" xfId="42"/>
+    <cellStyle name="Heading 5" xfId="43"/>
+    <cellStyle name="Heading1" xfId="44"/>
+    <cellStyle name="Hyperlink 10" xfId="45"/>
+    <cellStyle name="Hyperlink 11" xfId="46"/>
+    <cellStyle name="Neutral 13" xfId="47"/>
+    <cellStyle name="Neutral 14" xfId="48"/>
+    <cellStyle name="Note 8" xfId="49"/>
+    <cellStyle name="Note 9" xfId="50"/>
+    <cellStyle name="Result" xfId="51"/>
+    <cellStyle name="Result2" xfId="52"/>
+    <cellStyle name="Status 11" xfId="53"/>
+    <cellStyle name="Status 12" xfId="54"/>
+    <cellStyle name="Text 7" xfId="55"/>
+    <cellStyle name="Text 8" xfId="56"/>
+    <cellStyle name="Warning 15" xfId="57"/>
+    <cellStyle name="Warning 16" xfId="58"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="59"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="60"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="61"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Bad" xfId="62"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Neutral" xfId="63"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="64"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -4266,7 +4271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4303,7 +4308,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ27"/>
+  <dimension ref="A1:ALQ21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -4315,31 +4320,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="36.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="30.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="26.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="53.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="44.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="44.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="51.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="51.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1005" min="9" style="4" width="51.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="64.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="46.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="51.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="51.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1005" min="9" style="4" width="51.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1006" style="4" width="11.18"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="8" t="s">
@@ -7343,1277 +7348,601 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="2" s="15" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>1010</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>1011</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>1012</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>1013</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="n">
+        <v>517</v>
+      </c>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>1014</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="ALR2" s="4"/>
-      <c r="ALS2" s="4"/>
-      <c r="ALT2" s="4"/>
-      <c r="ALU2" s="4"/>
-      <c r="ALV2" s="4"/>
-      <c r="ALW2" s="4"/>
-      <c r="ALX2" s="4"/>
-      <c r="ALY2" s="4"/>
-      <c r="ALZ2" s="4"/>
-      <c r="AMA2" s="4"/>
-      <c r="AMB2" s="4"/>
-      <c r="AMC2" s="4"/>
-      <c r="AMD2" s="4"/>
-      <c r="AME2" s="4"/>
-      <c r="AMF2" s="4"/>
-      <c r="AMG2" s="4"/>
-      <c r="AMH2" s="4"/>
-      <c r="AMI2" s="4"/>
-      <c r="AMJ2" s="4"/>
+      <c r="B3" s="11" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="11" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
     </row>
-    <row r="3" s="15" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>1016</v>
-      </c>
-      <c r="D3" s="10" t="s">
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>1017</v>
       </c>
-      <c r="E3" s="17" t="n">
-        <v>517</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="ALR3" s="4"/>
-      <c r="ALS3" s="4"/>
-      <c r="ALT3" s="4"/>
-      <c r="ALU3" s="4"/>
-      <c r="ALV3" s="4"/>
-      <c r="ALW3" s="4"/>
-      <c r="ALX3" s="4"/>
-      <c r="ALY3" s="4"/>
-      <c r="ALZ3" s="4"/>
-      <c r="AMA3" s="4"/>
-      <c r="AMB3" s="4"/>
-      <c r="AMC3" s="4"/>
-      <c r="AMD3" s="4"/>
-      <c r="AME3" s="4"/>
-      <c r="AMF3" s="4"/>
-      <c r="AMG3" s="4"/>
-      <c r="AMH3" s="4"/>
-      <c r="AMI3" s="4"/>
-      <c r="AMJ3" s="4"/>
-    </row>
-    <row r="4" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="B4" s="11" t="s">
         <v>1018</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="12" t="s">
         <v>1019</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>1020</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>1021</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="ALR4" s="4"/>
-      <c r="ALS4" s="4"/>
-      <c r="ALT4" s="4"/>
-      <c r="ALU4" s="4"/>
-      <c r="ALV4" s="4"/>
-      <c r="ALW4" s="4"/>
-      <c r="ALX4" s="4"/>
-      <c r="ALY4" s="4"/>
-      <c r="ALZ4" s="4"/>
-      <c r="AMA4" s="4"/>
-      <c r="AMB4" s="4"/>
-      <c r="AMC4" s="4"/>
-      <c r="AMD4" s="4"/>
-      <c r="AME4" s="4"/>
-      <c r="AMF4" s="4"/>
-      <c r="AMG4" s="4"/>
-      <c r="AMH4" s="4"/>
-      <c r="AMI4" s="4"/>
-      <c r="AMJ4" s="4"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
     </row>
-    <row r="5" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+    <row r="5" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
         <v>1022</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>1023</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="15" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>1024</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="F5" s="0"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>1025</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="B6" s="15" t="s">
         <v>1026</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="ALR5" s="4"/>
-      <c r="ALS5" s="4"/>
-      <c r="ALT5" s="4"/>
-      <c r="ALU5" s="4"/>
-      <c r="ALV5" s="4"/>
-      <c r="ALW5" s="4"/>
-      <c r="ALX5" s="4"/>
-      <c r="ALY5" s="4"/>
-      <c r="ALZ5" s="4"/>
-      <c r="AMA5" s="4"/>
-      <c r="AMB5" s="4"/>
-      <c r="AMC5" s="4"/>
-      <c r="AMD5" s="4"/>
-      <c r="AME5" s="4"/>
-      <c r="AMF5" s="4"/>
-      <c r="AMG5" s="4"/>
-      <c r="AMH5" s="4"/>
-      <c r="AMI5" s="4"/>
-      <c r="AMJ5" s="4"/>
+      <c r="C6" s="15" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
     </row>
-    <row r="6" s="15" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B6" s="10" t="s">
+    <row r="7" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E7" s="17" t="n">
+        <v>81611</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E8" s="17" t="n">
+        <v>454909</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E9" s="17" t="n">
+        <v>52.0775912</v>
+      </c>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E10" s="17" t="n">
+        <v>4.3166395</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>1011</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>1028</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>1017</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>1029</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="ALR6" s="4"/>
-      <c r="ALS6" s="4"/>
-      <c r="ALT6" s="4"/>
-      <c r="ALU6" s="4"/>
-      <c r="ALV6" s="4"/>
-      <c r="ALW6" s="4"/>
-      <c r="ALX6" s="4"/>
-      <c r="ALY6" s="4"/>
-      <c r="ALZ6" s="4"/>
-      <c r="AMA6" s="4"/>
-      <c r="AMB6" s="4"/>
-      <c r="AMC6" s="4"/>
-      <c r="AMD6" s="4"/>
-      <c r="AME6" s="4"/>
-      <c r="AMF6" s="4"/>
-      <c r="AMG6" s="4"/>
-      <c r="AMH6" s="4"/>
-      <c r="AMI6" s="4"/>
-      <c r="AMJ6" s="4"/>
+      <c r="C14" s="12" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
     </row>
-    <row r="7" s="15" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
-        <v>1030</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>1031</v>
-      </c>
-      <c r="D7" s="10" t="s">
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="25" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="28" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>1020</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>1032</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="ALR7" s="4"/>
-      <c r="ALS7" s="4"/>
-      <c r="ALT7" s="4"/>
-      <c r="ALU7" s="4"/>
-      <c r="ALV7" s="4"/>
-      <c r="ALW7" s="4"/>
-      <c r="ALX7" s="4"/>
-      <c r="ALY7" s="4"/>
-      <c r="ALZ7" s="4"/>
-      <c r="AMA7" s="4"/>
-      <c r="AMB7" s="4"/>
-      <c r="AMC7" s="4"/>
-      <c r="AMD7" s="4"/>
-      <c r="AME7" s="4"/>
-      <c r="AMF7" s="4"/>
-      <c r="AMG7" s="4"/>
-      <c r="AMH7" s="4"/>
-      <c r="AMI7" s="4"/>
-      <c r="AMJ7" s="4"/>
-    </row>
-    <row r="8" s="15" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>1035</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>1036</v>
-      </c>
-      <c r="E8" s="19" t="n">
-        <v>81611</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="ALR8" s="4"/>
-      <c r="ALS8" s="4"/>
-      <c r="ALT8" s="4"/>
-      <c r="ALU8" s="4"/>
-      <c r="ALV8" s="4"/>
-      <c r="ALW8" s="4"/>
-      <c r="ALX8" s="4"/>
-      <c r="ALY8" s="4"/>
-      <c r="ALZ8" s="4"/>
-      <c r="AMA8" s="4"/>
-      <c r="AMB8" s="4"/>
-      <c r="AMC8" s="4"/>
-      <c r="AMD8" s="4"/>
-      <c r="AME8" s="4"/>
-      <c r="AMF8" s="4"/>
-      <c r="AMG8" s="4"/>
-      <c r="AMH8" s="4"/>
-      <c r="AMI8" s="4"/>
-      <c r="AMJ8" s="4"/>
-    </row>
-    <row r="9" s="15" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
-        <v>1011</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>1037</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>1038</v>
-      </c>
-      <c r="E9" s="19" t="n">
-        <v>454909</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="ALR9" s="4"/>
-      <c r="ALS9" s="4"/>
-      <c r="ALT9" s="4"/>
-      <c r="ALU9" s="4"/>
-      <c r="ALV9" s="4"/>
-      <c r="ALW9" s="4"/>
-      <c r="ALX9" s="4"/>
-      <c r="ALY9" s="4"/>
-      <c r="ALZ9" s="4"/>
-      <c r="AMA9" s="4"/>
-      <c r="AMB9" s="4"/>
-      <c r="AMC9" s="4"/>
-      <c r="AMD9" s="4"/>
-      <c r="AME9" s="4"/>
-      <c r="AMF9" s="4"/>
-      <c r="AMG9" s="4"/>
-      <c r="AMH9" s="4"/>
-      <c r="AMI9" s="4"/>
-      <c r="AMJ9" s="4"/>
-    </row>
-    <row r="10" s="15" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>1040</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E10" s="19" t="n">
-        <v>4.3166395</v>
-      </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="ALR10" s="4"/>
-      <c r="ALS10" s="4"/>
-      <c r="ALT10" s="4"/>
-      <c r="ALU10" s="4"/>
-      <c r="ALV10" s="4"/>
-      <c r="ALW10" s="4"/>
-      <c r="ALX10" s="4"/>
-      <c r="ALY10" s="4"/>
-      <c r="ALZ10" s="4"/>
-      <c r="AMA10" s="4"/>
-      <c r="AMB10" s="4"/>
-      <c r="AMC10" s="4"/>
-      <c r="AMD10" s="4"/>
-      <c r="AME10" s="4"/>
-      <c r="AMF10" s="4"/>
-      <c r="AMG10" s="4"/>
-      <c r="AMH10" s="4"/>
-      <c r="AMI10" s="4"/>
-      <c r="AMJ10" s="4"/>
-    </row>
-    <row r="11" s="15" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
-        <v>1042</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>1034</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>1043</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E11" s="19" t="n">
-        <v>52.0775912</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="ALR11" s="4"/>
-      <c r="ALS11" s="4"/>
-      <c r="ALT11" s="4"/>
-      <c r="ALU11" s="4"/>
-      <c r="ALV11" s="4"/>
-      <c r="ALW11" s="4"/>
-      <c r="ALX11" s="4"/>
-      <c r="ALY11" s="4"/>
-      <c r="ALZ11" s="4"/>
-      <c r="AMA11" s="4"/>
-      <c r="AMB11" s="4"/>
-      <c r="AMC11" s="4"/>
-      <c r="AMD11" s="4"/>
-      <c r="AME11" s="4"/>
-      <c r="AMF11" s="4"/>
-      <c r="AMG11" s="4"/>
-      <c r="AMH11" s="4"/>
-      <c r="AMI11" s="4"/>
-      <c r="AMJ11" s="4"/>
-    </row>
-    <row r="12" s="15" customFormat="true" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
-        <v>1044</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>1046</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>1048</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="ALR12" s="4"/>
-      <c r="ALS12" s="4"/>
-      <c r="ALT12" s="4"/>
-      <c r="ALU12" s="4"/>
-      <c r="ALV12" s="4"/>
-      <c r="ALW12" s="4"/>
-      <c r="ALX12" s="4"/>
-      <c r="ALY12" s="4"/>
-      <c r="ALZ12" s="4"/>
-      <c r="AMA12" s="4"/>
-      <c r="AMB12" s="4"/>
-      <c r="AMC12" s="4"/>
-      <c r="AMD12" s="4"/>
-      <c r="AME12" s="4"/>
-      <c r="AMF12" s="4"/>
-      <c r="AMG12" s="4"/>
-      <c r="AMH12" s="4"/>
-      <c r="AMI12" s="4"/>
-      <c r="AMJ12" s="4"/>
-    </row>
-    <row r="13" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
-        <v>1049</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>1052</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="ALR13" s="4"/>
-      <c r="ALS13" s="4"/>
-      <c r="ALT13" s="4"/>
-      <c r="ALU13" s="4"/>
-      <c r="ALV13" s="4"/>
-      <c r="ALW13" s="4"/>
-      <c r="ALX13" s="4"/>
-      <c r="ALY13" s="4"/>
-      <c r="ALZ13" s="4"/>
-      <c r="AMA13" s="4"/>
-      <c r="AMB13" s="4"/>
-      <c r="AMC13" s="4"/>
-      <c r="AMD13" s="4"/>
-      <c r="AME13" s="4"/>
-      <c r="AMF13" s="4"/>
-      <c r="AMG13" s="4"/>
-      <c r="AMH13" s="4"/>
-      <c r="AMI13" s="4"/>
-      <c r="AMJ13" s="4"/>
-    </row>
-    <row r="14" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
-        <v>1053</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>1054</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="ALR14" s="4"/>
-      <c r="ALS14" s="4"/>
-      <c r="ALT14" s="4"/>
-      <c r="ALU14" s="4"/>
-      <c r="ALV14" s="4"/>
-      <c r="ALW14" s="4"/>
-      <c r="ALX14" s="4"/>
-      <c r="ALY14" s="4"/>
-      <c r="ALZ14" s="4"/>
-      <c r="AMA14" s="4"/>
-      <c r="AMB14" s="4"/>
-      <c r="AMC14" s="4"/>
-      <c r="AMD14" s="4"/>
-      <c r="AME14" s="4"/>
-      <c r="AMF14" s="4"/>
-      <c r="AMG14" s="4"/>
-      <c r="AMH14" s="4"/>
-      <c r="AMI14" s="4"/>
-      <c r="AMJ14" s="4"/>
-    </row>
-    <row r="15" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>1056</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="ALR15" s="4"/>
-      <c r="ALS15" s="4"/>
-      <c r="ALT15" s="4"/>
-      <c r="ALU15" s="4"/>
-      <c r="ALV15" s="4"/>
-      <c r="ALW15" s="4"/>
-      <c r="ALX15" s="4"/>
-      <c r="ALY15" s="4"/>
-      <c r="ALZ15" s="4"/>
-      <c r="AMA15" s="4"/>
-      <c r="AMB15" s="4"/>
-      <c r="AMC15" s="4"/>
-      <c r="AMD15" s="4"/>
-      <c r="AME15" s="4"/>
-      <c r="AMF15" s="4"/>
-      <c r="AMG15" s="4"/>
-      <c r="AMH15" s="4"/>
-      <c r="AMI15" s="4"/>
-      <c r="AMJ15" s="4"/>
-    </row>
-    <row r="16" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
-        <v>1057</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>1058</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="ALR16" s="4"/>
-      <c r="ALS16" s="4"/>
-      <c r="ALT16" s="4"/>
-      <c r="ALU16" s="4"/>
-      <c r="ALV16" s="4"/>
-      <c r="ALW16" s="4"/>
-      <c r="ALX16" s="4"/>
-      <c r="ALY16" s="4"/>
-      <c r="ALZ16" s="4"/>
-      <c r="AMA16" s="4"/>
-      <c r="AMB16" s="4"/>
-      <c r="AMC16" s="4"/>
-      <c r="AMD16" s="4"/>
-      <c r="AME16" s="4"/>
-      <c r="AMF16" s="4"/>
-      <c r="AMG16" s="4"/>
-      <c r="AMH16" s="4"/>
-      <c r="AMI16" s="4"/>
-      <c r="AMJ16" s="4"/>
-    </row>
-    <row r="17" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
-        <v>1059</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>1060</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>1061</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="ALR17" s="4"/>
-      <c r="ALS17" s="4"/>
-      <c r="ALT17" s="4"/>
-      <c r="ALU17" s="4"/>
-      <c r="ALV17" s="4"/>
-      <c r="ALW17" s="4"/>
-      <c r="ALX17" s="4"/>
-      <c r="ALY17" s="4"/>
-      <c r="ALZ17" s="4"/>
-      <c r="AMA17" s="4"/>
-      <c r="AMB17" s="4"/>
-      <c r="AMC17" s="4"/>
-      <c r="AMD17" s="4"/>
-      <c r="AME17" s="4"/>
-      <c r="AMF17" s="4"/>
-      <c r="AMG17" s="4"/>
-      <c r="AMH17" s="4"/>
-      <c r="AMI17" s="4"/>
-      <c r="AMJ17" s="4"/>
-    </row>
-    <row r="18" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
-        <v>1062</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>1063</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>1064</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="ALR18" s="4"/>
-      <c r="ALS18" s="4"/>
-      <c r="ALT18" s="4"/>
-      <c r="ALU18" s="4"/>
-      <c r="ALV18" s="4"/>
-      <c r="ALW18" s="4"/>
-      <c r="ALX18" s="4"/>
-      <c r="ALY18" s="4"/>
-      <c r="ALZ18" s="4"/>
-      <c r="AMA18" s="4"/>
-      <c r="AMB18" s="4"/>
-      <c r="AMC18" s="4"/>
-      <c r="AMD18" s="4"/>
-      <c r="AME18" s="4"/>
-      <c r="AMF18" s="4"/>
-      <c r="AMG18" s="4"/>
-      <c r="AMH18" s="4"/>
-      <c r="AMI18" s="4"/>
-      <c r="AMJ18" s="4"/>
-    </row>
-    <row r="19" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
-        <v>1065</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>1063</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>1047</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>1066</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="ALR19" s="4"/>
-      <c r="ALS19" s="4"/>
-      <c r="ALT19" s="4"/>
-      <c r="ALU19" s="4"/>
-      <c r="ALV19" s="4"/>
-      <c r="ALW19" s="4"/>
-      <c r="ALX19" s="4"/>
-      <c r="ALY19" s="4"/>
-      <c r="ALZ19" s="4"/>
-      <c r="AMA19" s="4"/>
-      <c r="AMB19" s="4"/>
-      <c r="AMC19" s="4"/>
-      <c r="AMD19" s="4"/>
-      <c r="AME19" s="4"/>
-      <c r="AMF19" s="4"/>
-      <c r="AMG19" s="4"/>
-      <c r="AMH19" s="4"/>
-      <c r="AMI19" s="4"/>
-      <c r="AMJ19" s="4"/>
-    </row>
-    <row r="20" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
-        <v>1067</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>1068</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>1011</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="ALR20" s="4"/>
-      <c r="ALS20" s="4"/>
-      <c r="ALT20" s="4"/>
-      <c r="ALU20" s="4"/>
-      <c r="ALV20" s="4"/>
-      <c r="ALW20" s="4"/>
-      <c r="ALX20" s="4"/>
-      <c r="ALY20" s="4"/>
-      <c r="ALZ20" s="4"/>
-      <c r="AMA20" s="4"/>
-      <c r="AMB20" s="4"/>
-      <c r="AMC20" s="4"/>
-      <c r="AMD20" s="4"/>
-      <c r="AME20" s="4"/>
-      <c r="AMF20" s="4"/>
-      <c r="AMG20" s="4"/>
-      <c r="AMH20" s="4"/>
-      <c r="AMI20" s="4"/>
-      <c r="AMJ20" s="4"/>
-    </row>
-    <row r="21" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
-        <v>1070</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>1071</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>1023</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="ALR21" s="4"/>
-      <c r="ALS21" s="4"/>
-      <c r="ALT21" s="4"/>
-      <c r="ALU21" s="4"/>
-      <c r="ALV21" s="4"/>
-      <c r="ALW21" s="4"/>
-      <c r="ALX21" s="4"/>
-      <c r="ALY21" s="4"/>
-      <c r="ALZ21" s="4"/>
-      <c r="AMA21" s="4"/>
-      <c r="AMB21" s="4"/>
-      <c r="AMC21" s="4"/>
-      <c r="AMD21" s="4"/>
-      <c r="AME21" s="4"/>
-      <c r="AMF21" s="4"/>
-      <c r="AMG21" s="4"/>
-      <c r="AMH21" s="4"/>
-      <c r="AMI21" s="4"/>
-      <c r="AMJ21" s="4"/>
-    </row>
-    <row r="22" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
+      <c r="E21" s="29" t="s">
         <v>1072</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>1073</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>1074</v>
-      </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="ALR22" s="4"/>
-      <c r="ALS22" s="4"/>
-      <c r="ALT22" s="4"/>
-      <c r="ALU22" s="4"/>
-      <c r="ALV22" s="4"/>
-      <c r="ALW22" s="4"/>
-      <c r="ALX22" s="4"/>
-      <c r="ALY22" s="4"/>
-      <c r="ALZ22" s="4"/>
-      <c r="AMA22" s="4"/>
-      <c r="AMB22" s="4"/>
-      <c r="AMC22" s="4"/>
-      <c r="AMD22" s="4"/>
-      <c r="AME22" s="4"/>
-      <c r="AMF22" s="4"/>
-      <c r="AMG22" s="4"/>
-      <c r="AMH22" s="4"/>
-      <c r="AMI22" s="4"/>
-      <c r="AMJ22" s="4"/>
-    </row>
-    <row r="23" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
-        <v>1075</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>1076</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>1077</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="ALR23" s="4"/>
-      <c r="ALS23" s="4"/>
-      <c r="ALT23" s="4"/>
-      <c r="ALU23" s="4"/>
-      <c r="ALV23" s="4"/>
-      <c r="ALW23" s="4"/>
-      <c r="ALX23" s="4"/>
-      <c r="ALY23" s="4"/>
-      <c r="ALZ23" s="4"/>
-      <c r="AMA23" s="4"/>
-      <c r="AMB23" s="4"/>
-      <c r="AMC23" s="4"/>
-      <c r="AMD23" s="4"/>
-      <c r="AME23" s="4"/>
-      <c r="AMF23" s="4"/>
-      <c r="AMG23" s="4"/>
-      <c r="AMH23" s="4"/>
-      <c r="AMI23" s="4"/>
-      <c r="AMJ23" s="4"/>
-    </row>
-    <row r="24" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
-        <v>1078</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>1079</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>1011</v>
-      </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="ALR24" s="4"/>
-      <c r="ALS24" s="4"/>
-      <c r="ALT24" s="4"/>
-      <c r="ALU24" s="4"/>
-      <c r="ALV24" s="4"/>
-      <c r="ALW24" s="4"/>
-      <c r="ALX24" s="4"/>
-      <c r="ALY24" s="4"/>
-      <c r="ALZ24" s="4"/>
-      <c r="AMA24" s="4"/>
-      <c r="AMB24" s="4"/>
-      <c r="AMC24" s="4"/>
-      <c r="AMD24" s="4"/>
-      <c r="AME24" s="4"/>
-      <c r="AMF24" s="4"/>
-      <c r="AMG24" s="4"/>
-      <c r="AMH24" s="4"/>
-      <c r="AMI24" s="4"/>
-      <c r="AMJ24" s="4"/>
-    </row>
-    <row r="25" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>1081</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>1011</v>
-      </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="ALR25" s="4"/>
-      <c r="ALS25" s="4"/>
-      <c r="ALT25" s="4"/>
-      <c r="ALU25" s="4"/>
-      <c r="ALV25" s="4"/>
-      <c r="ALW25" s="4"/>
-      <c r="ALX25" s="4"/>
-      <c r="ALY25" s="4"/>
-      <c r="ALZ25" s="4"/>
-      <c r="AMA25" s="4"/>
-      <c r="AMB25" s="4"/>
-      <c r="AMC25" s="4"/>
-      <c r="AMD25" s="4"/>
-      <c r="AME25" s="4"/>
-      <c r="AMF25" s="4"/>
-      <c r="AMG25" s="4"/>
-      <c r="AMH25" s="4"/>
-      <c r="AMI25" s="4"/>
-      <c r="AMJ25" s="4"/>
-    </row>
-    <row r="26" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="26" t="s">
-        <v>1082</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>1085</v>
-      </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="ALR26" s="4"/>
-      <c r="ALS26" s="4"/>
-      <c r="ALT26" s="4"/>
-      <c r="ALU26" s="4"/>
-      <c r="ALV26" s="4"/>
-      <c r="ALW26" s="4"/>
-      <c r="ALX26" s="4"/>
-      <c r="ALY26" s="4"/>
-      <c r="ALZ26" s="4"/>
-      <c r="AMA26" s="4"/>
-      <c r="AMB26" s="4"/>
-      <c r="AMC26" s="4"/>
-      <c r="AMD26" s="4"/>
-      <c r="AME26" s="4"/>
-      <c r="AMF26" s="4"/>
-      <c r="AMG26" s="4"/>
-      <c r="AMH26" s="4"/>
-      <c r="AMI26" s="4"/>
-      <c r="AMJ26" s="4"/>
-    </row>
-    <row r="27" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="26" t="s">
-        <v>1086</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>1011</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>1087</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>1025</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>1088</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="ALR27" s="4"/>
-      <c r="ALS27" s="4"/>
-      <c r="ALT27" s="4"/>
-      <c r="ALU27" s="4"/>
-      <c r="ALV27" s="4"/>
-      <c r="ALW27" s="4"/>
-      <c r="ALX27" s="4"/>
-      <c r="ALY27" s="4"/>
-      <c r="ALZ27" s="4"/>
-      <c r="AMA27" s="4"/>
-      <c r="AMB27" s="4"/>
-      <c r="AMC27" s="4"/>
-      <c r="AMD27" s="4"/>
-      <c r="AME27" s="4"/>
-      <c r="AMF27" s="4"/>
-      <c r="AMG27" s="4"/>
-      <c r="AMH27" s="4"/>
-      <c r="AMI27" s="4"/>
-      <c r="AMJ27" s="4"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -8641,597 +7970,597 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="70.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="79.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="27" width="69.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="27" width="75.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="27" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="70.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="79.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="69.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="26" width="75.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="26" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="31"/>
+      <c r="E1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34" t="s">
-        <v>1090</v>
-      </c>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="36" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>1011</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>1091</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>1093</v>
-      </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="38" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="31"/>
+      <c r="I2" s="14"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
     </row>
-    <row r="3" s="4" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>1094</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>1095</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>1096</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>1093</v>
+    <row r="3" s="4" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>1080</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
-        <v>1097</v>
-      </c>
-      <c r="B4" s="33" t="s">
+      <c r="A4" s="39" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B4" s="35" t="s">
         <v>1011</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1098</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>1099</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>1093</v>
+        <v>1082</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>1084</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="37" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B5" s="38" t="s">
+      <c r="A5" s="39" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>1011</v>
       </c>
-      <c r="C5" s="39" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>1102</v>
+      <c r="C5" s="41" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>1087</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
-        <v>1103</v>
-      </c>
-      <c r="B6" s="38" t="s">
+      <c r="A6" s="39" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B6" s="40" t="s">
         <v>1011</v>
       </c>
-      <c r="C6" s="39" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>1104</v>
-      </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
+      <c r="C6" s="41" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
-        <v>1105</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>1106</v>
-      </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
+      <c r="A7" s="39" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
-        <v>1107</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>1108</v>
-      </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
+      <c r="A8" s="39" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37" t="s">
-        <v>1109</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>1023</v>
+      <c r="A9" s="39" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>1018</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>1111</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>1093</v>
+        <v>1095</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>1097</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="31"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="s">
-        <v>1112</v>
-      </c>
-      <c r="B10" s="38" t="s">
+      <c r="A10" s="39" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B10" s="40" t="s">
         <v>1011</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41" t="s">
-        <v>1113</v>
-      </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
+      <c r="C10" s="41" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="s">
-        <v>1114</v>
-      </c>
-      <c r="B11" s="38" t="s">
+      <c r="A11" s="39" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B11" s="40" t="s">
         <v>1011</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="41" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43" t="s">
         <v>1101</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41" t="s">
-        <v>1115</v>
-      </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="31"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>1093</v>
+      <c r="A12" s="39" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>1105</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B13" s="33" t="s">
+      <c r="A13" s="39" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B13" s="35" t="s">
         <v>1011</v>
       </c>
-      <c r="C13" s="32" t="s">
-        <v>1120</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>1121</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>1093</v>
-      </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
+      <c r="C13" s="34" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42" t="s">
-        <v>1123</v>
-      </c>
-      <c r="F14" s="31"/>
+      <c r="A14" s="39" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F14" s="14"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="s">
-        <v>1124</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>1125</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>1126</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>1093</v>
-      </c>
-      <c r="F15" s="31"/>
+      <c r="A15" s="39" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>1115</v>
+      </c>
+      <c r="F15" s="14"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="31"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="14"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37" t="s">
-        <v>1127</v>
-      </c>
-      <c r="B16" s="33" t="s">
+      <c r="A16" s="39" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B16" s="35" t="s">
         <v>1011</v>
       </c>
-      <c r="C16" s="32" t="s">
-        <v>1128</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>1129</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>1130</v>
-      </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="31"/>
+      <c r="C16" s="34" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37" t="s">
-        <v>1131</v>
-      </c>
-      <c r="B17" s="33" t="s">
+      <c r="A17" s="39" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B17" s="35" t="s">
         <v>1011</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>1132</v>
-      </c>
-      <c r="D17" s="32" t="s">
+      <c r="C17" s="34" t="s">
         <v>1121</v>
       </c>
-      <c r="E17" s="31" t="s">
-        <v>1093</v>
-      </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="31"/>
+      <c r="D17" s="34" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37" t="s">
-        <v>1133</v>
-      </c>
-      <c r="B18" s="38" t="s">
+      <c r="A18" s="39" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B18" s="40" t="s">
         <v>1011</v>
       </c>
-      <c r="C18" s="39" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45" t="s">
-        <v>1134</v>
-      </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="31"/>
+      <c r="C18" s="41" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="14"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="37" t="s">
-        <v>1135</v>
-      </c>
-      <c r="B19" s="38" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>1136</v>
-      </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="40" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F19" s="31"/>
+      <c r="A19" s="39" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D19" s="45"/>
+      <c r="E19" s="42" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F19" s="14"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="31"/>
+      <c r="I19" s="14"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
-        <v>1138</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>1139</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>1140</v>
-      </c>
-      <c r="E20" s="31" t="s">
-        <v>1093</v>
-      </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
+      <c r="A20" s="39" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B21" s="27" t="s">
+      <c r="A21" s="25" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B21" s="26" t="s">
         <v>1011</v>
       </c>
-      <c r="C21" s="47" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>1143</v>
+      <c r="C21" s="49" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>1133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some small fixes in tests
</commit_message>
<xml_diff>
--- a/files/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/files/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -3465,7 +3465,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3639,12 +3639,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
@@ -3790,7 +3784,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -3919,14 +3913,14 @@
     <xf numFmtId="164" fontId="23" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3979,127 +3973,135 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7339,7 +7341,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="15" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>1010</v>
       </c>
@@ -7356,18 +7358,18 @@
         <v>517</v>
       </c>
       <c r="F2" s="13"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
       <c r="ALR2" s="4"/>
       <c r="ALS2" s="4"/>
       <c r="ALT2" s="4"/>
@@ -7388,7 +7390,7 @@
       <c r="AMI2" s="4"/>
       <c r="AMJ2" s="4"/>
     </row>
-    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>1014</v>
       </c>
@@ -7402,19 +7404,19 @@
       <c r="E3" s="12" t="s">
         <v>1016</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
       <c r="ALR3" s="4"/>
       <c r="ALS3" s="4"/>
       <c r="ALT3" s="4"/>
@@ -7435,7 +7437,7 @@
       <c r="AMI3" s="4"/>
       <c r="AMJ3" s="4"/>
     </row>
-    <row r="4" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>1017</v>
       </c>
@@ -7448,22 +7450,22 @@
       <c r="D4" s="10" t="s">
         <v>1020</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="17" t="s">
         <v>1021</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
       <c r="ALR4" s="4"/>
       <c r="ALS4" s="4"/>
       <c r="ALT4" s="4"/>
@@ -7484,7 +7486,7 @@
       <c r="AMI4" s="4"/>
       <c r="AMJ4" s="4"/>
     </row>
-    <row r="5" s="5" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="15" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>1022</v>
       </c>
@@ -7497,22 +7499,22 @@
       <c r="D5" s="10" t="s">
         <v>1013</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="13" t="s">
         <v>1024</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
       <c r="ALR5" s="4"/>
       <c r="ALS5" s="4"/>
       <c r="ALT5" s="4"/>
@@ -7533,35 +7535,35 @@
       <c r="AMI5" s="4"/>
       <c r="AMJ5" s="4"/>
     </row>
-    <row r="6" s="5" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="15" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>1025</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>1026</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="10" t="s">
         <v>1027</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>1015</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="19" t="s">
         <v>1028</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
       <c r="ALR6" s="4"/>
       <c r="ALS6" s="4"/>
       <c r="ALT6" s="4"/>
@@ -7582,7 +7584,7 @@
       <c r="AMI6" s="4"/>
       <c r="AMJ6" s="4"/>
     </row>
-    <row r="7" s="5" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="15" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>1029</v>
       </c>
@@ -7595,22 +7597,22 @@
       <c r="D7" s="10" t="s">
         <v>1032</v>
       </c>
-      <c r="E7" s="13" t="n">
+      <c r="E7" s="17" t="n">
         <v>81611</v>
       </c>
       <c r="F7" s="13"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
       <c r="ALR7" s="4"/>
       <c r="ALS7" s="4"/>
       <c r="ALT7" s="4"/>
@@ -7631,7 +7633,7 @@
       <c r="AMI7" s="4"/>
       <c r="AMJ7" s="4"/>
     </row>
-    <row r="8" s="5" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="15" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>1033</v>
       </c>
@@ -7644,22 +7646,22 @@
       <c r="D8" s="10" t="s">
         <v>1035</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="17" t="n">
         <v>454909</v>
       </c>
       <c r="F8" s="13"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
       <c r="ALR8" s="4"/>
       <c r="ALS8" s="4"/>
       <c r="ALT8" s="4"/>
@@ -7680,7 +7682,7 @@
       <c r="AMI8" s="4"/>
       <c r="AMJ8" s="4"/>
     </row>
-    <row r="9" s="5" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="15" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>1036</v>
       </c>
@@ -7693,22 +7695,22 @@
       <c r="D9" s="11" t="s">
         <v>1038</v>
       </c>
-      <c r="E9" s="13" t="n">
+      <c r="E9" s="17" t="n">
         <v>52.0775912</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
       <c r="ALR9" s="4"/>
       <c r="ALS9" s="4"/>
       <c r="ALT9" s="4"/>
@@ -7729,7 +7731,7 @@
       <c r="AMI9" s="4"/>
       <c r="AMJ9" s="4"/>
     </row>
-    <row r="10" s="5" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="15" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
         <v>1039</v>
       </c>
@@ -7742,22 +7744,22 @@
       <c r="D10" s="11" t="s">
         <v>1038</v>
       </c>
-      <c r="E10" s="13" t="n">
+      <c r="E10" s="17" t="n">
         <v>4.3166395</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
       <c r="ALR10" s="4"/>
       <c r="ALS10" s="4"/>
       <c r="ALT10" s="4"/>
@@ -7778,7 +7780,7 @@
       <c r="AMI10" s="4"/>
       <c r="AMJ10" s="4"/>
     </row>
-    <row r="11" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>1041</v>
       </c>
@@ -7791,22 +7793,22 @@
       <c r="D11" s="10" t="s">
         <v>1044</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>1045</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
       <c r="ALR11" s="4"/>
       <c r="ALS11" s="4"/>
       <c r="ALT11" s="4"/>
@@ -7827,7 +7829,7 @@
       <c r="AMI11" s="4"/>
       <c r="AMJ11" s="4"/>
     </row>
-    <row r="12" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
         <v>1046</v>
       </c>
@@ -7840,22 +7842,22 @@
       <c r="D12" s="10" t="s">
         <v>1044</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="13" t="s">
         <v>1047</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
       <c r="ALR12" s="4"/>
       <c r="ALS12" s="4"/>
       <c r="ALT12" s="4"/>
@@ -7876,7 +7878,7 @@
       <c r="AMI12" s="4"/>
       <c r="AMJ12" s="4"/>
     </row>
-    <row r="13" s="5" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="15" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
         <v>1048</v>
       </c>
@@ -7889,22 +7891,22 @@
       <c r="D13" s="10" t="s">
         <v>1044</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="13" t="s">
         <v>1050</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
       <c r="ALR13" s="4"/>
       <c r="ALS13" s="4"/>
       <c r="ALT13" s="4"/>
@@ -7925,7 +7927,7 @@
       <c r="AMI13" s="4"/>
       <c r="AMJ13" s="4"/>
     </row>
-    <row r="14" s="5" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="15" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>1051</v>
       </c>
@@ -7938,20 +7940,20 @@
       <c r="D14" s="10" t="s">
         <v>1053</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="17" t="s">
         <v>1011</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
       <c r="ALR14" s="4"/>
       <c r="ALS14" s="4"/>
       <c r="ALT14" s="4"/>
@@ -7972,7 +7974,7 @@
       <c r="AMI14" s="4"/>
       <c r="AMJ14" s="4"/>
     </row>
-    <row r="15" s="5" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
         <v>1054</v>
       </c>
@@ -7985,22 +7987,22 @@
       <c r="D15" s="10" t="s">
         <v>1053</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="17" t="s">
         <v>1018</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
       <c r="ALR15" s="4"/>
       <c r="ALS15" s="4"/>
       <c r="ALT15" s="4"/>
@@ -8021,7 +8023,7 @@
       <c r="AMI15" s="4"/>
       <c r="AMJ15" s="4"/>
     </row>
-    <row r="16" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
         <v>1056</v>
       </c>
@@ -8034,22 +8036,22 @@
       <c r="D16" s="10" t="s">
         <v>1015</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="17" t="s">
         <v>1058</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
       <c r="ALR16" s="4"/>
       <c r="ALS16" s="4"/>
       <c r="ALT16" s="4"/>
@@ -8070,7 +8072,7 @@
       <c r="AMI16" s="4"/>
       <c r="AMJ16" s="4"/>
     </row>
-    <row r="17" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
         <v>1059</v>
       </c>
@@ -8083,22 +8085,22 @@
       <c r="D17" s="10" t="s">
         <v>1015</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="17" t="s">
         <v>1061</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
       <c r="ALR17" s="4"/>
       <c r="ALS17" s="4"/>
       <c r="ALT17" s="4"/>
@@ -8119,7 +8121,7 @@
       <c r="AMI17" s="4"/>
       <c r="AMJ17" s="4"/>
     </row>
-    <row r="18" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
         <v>1062</v>
       </c>
@@ -8132,22 +8134,22 @@
       <c r="D18" s="10" t="s">
         <v>1053</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="17" t="s">
         <v>1011</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
       <c r="ALR18" s="4"/>
       <c r="ALS18" s="4"/>
       <c r="ALT18" s="4"/>
@@ -8168,7 +8170,7 @@
       <c r="AMI18" s="4"/>
       <c r="AMJ18" s="4"/>
     </row>
-    <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
         <v>1064</v>
       </c>
@@ -8184,19 +8186,19 @@
       <c r="E19" s="21" t="s">
         <v>1011</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
       <c r="ALR19" s="4"/>
       <c r="ALS19" s="4"/>
       <c r="ALT19" s="4"/>
@@ -8217,7 +8219,7 @@
       <c r="AMI19" s="4"/>
       <c r="AMJ19" s="4"/>
     </row>
-    <row r="20" s="5" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
         <v>1066</v>
       </c>
@@ -8233,19 +8235,19 @@
       <c r="E20" s="23" t="s">
         <v>1069</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
       <c r="ALR20" s="4"/>
       <c r="ALS20" s="4"/>
       <c r="ALT20" s="4"/>
@@ -8266,7 +8268,7 @@
       <c r="AMI20" s="4"/>
       <c r="AMJ20" s="4"/>
     </row>
-    <row r="21" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
         <v>1070</v>
       </c>
@@ -8283,18 +8285,18 @@
         <v>1072</v>
       </c>
       <c r="F21" s="24"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
       <c r="ALR21" s="4"/>
       <c r="ALS21" s="4"/>
       <c r="ALT21" s="4"/>
@@ -8433,7 +8435,7 @@
       <c r="D4" s="30" t="s">
         <v>1083</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="37" t="s">
         <v>1084</v>
       </c>
       <c r="F4" s="1"/>
@@ -8454,16 +8456,16 @@
       <c r="A5" s="36" t="s">
         <v>1085</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="39" t="s">
         <v>1086</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="40" t="s">
         <v>1015</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="40" t="s">
         <v>1087</v>
       </c>
       <c r="F5" s="1"/>
@@ -8484,16 +8486,16 @@
       <c r="A6" s="36" t="s">
         <v>1088</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="39" t="s">
         <v>1086</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="41" t="s">
         <v>1015</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="41" t="s">
         <v>1089</v>
       </c>
       <c r="F6" s="29"/>
@@ -8514,16 +8516,16 @@
       <c r="A7" s="36" t="s">
         <v>1090</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="38" t="s">
         <v>1018</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="39" t="s">
         <v>1086</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="41" t="s">
         <v>1015</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="41" t="s">
         <v>1091</v>
       </c>
       <c r="F7" s="29"/>
@@ -8544,16 +8546,16 @@
       <c r="A8" s="36" t="s">
         <v>1092</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="38" t="s">
         <v>1018</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="39" t="s">
         <v>1086</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="41" t="s">
         <v>1015</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="41" t="s">
         <v>1093</v>
       </c>
       <c r="F8" s="29"/>
@@ -8583,7 +8585,7 @@
       <c r="D9" s="30" t="s">
         <v>1096</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="37" t="s">
         <v>1097</v>
       </c>
       <c r="F9" s="1"/>
@@ -8604,14 +8606,14 @@
       <c r="A10" s="36" t="s">
         <v>1098</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="39" t="s">
         <v>1086</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40" t="s">
+      <c r="D10" s="41"/>
+      <c r="E10" s="41" t="s">
         <v>1099</v>
       </c>
       <c r="F10" s="29"/>
@@ -8632,14 +8634,14 @@
       <c r="A11" s="36" t="s">
         <v>1100</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="39" t="s">
         <v>1086</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40" t="s">
+      <c r="D11" s="41"/>
+      <c r="E11" s="41" t="s">
         <v>1101</v>
       </c>
       <c r="F11" s="34"/>
@@ -8669,7 +8671,7 @@
       <c r="D12" s="30" t="s">
         <v>1104</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="37" t="s">
         <v>1105</v>
       </c>
       <c r="F12" s="1"/>
@@ -8699,7 +8701,7 @@
       <c r="D13" s="30" t="s">
         <v>1108</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="42" t="s">
         <v>1109</v>
       </c>
       <c r="F13" s="29"/>
@@ -8720,14 +8722,14 @@
       <c r="A14" s="36" t="s">
         <v>1110</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="38" t="s">
         <v>1018</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="39" t="s">
         <v>1086</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42" t="s">
+      <c r="D14" s="43"/>
+      <c r="E14" s="43" t="s">
         <v>1111</v>
       </c>
       <c r="F14" s="29"/>
@@ -8757,12 +8759,12 @@
       <c r="D15" s="30" t="s">
         <v>1114</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="18" t="s">
         <v>1115</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="16"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="29"/>
       <c r="J15" s="1"/>
       <c r="K15" s="29"/>
@@ -8784,15 +8786,15 @@
       <c r="C16" s="30" t="s">
         <v>1117</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="45" t="s">
         <v>1118</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="45" t="s">
         <v>1119</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="16"/>
+      <c r="H16" s="44"/>
       <c r="I16" s="29"/>
       <c r="J16" s="1"/>
       <c r="K16" s="29"/>
@@ -8817,12 +8819,12 @@
       <c r="D17" s="30" t="s">
         <v>1108</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="42" t="s">
         <v>1109</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
-      <c r="H17" s="16"/>
+      <c r="H17" s="44"/>
       <c r="I17" s="29"/>
       <c r="J17" s="1"/>
       <c r="K17" s="29"/>
@@ -8838,19 +8840,19 @@
       <c r="A18" s="36" t="s">
         <v>1122</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="39" t="s">
         <v>1086</v>
       </c>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44" t="s">
+      <c r="D18" s="46"/>
+      <c r="E18" s="46" t="s">
         <v>1123</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="16"/>
+      <c r="H18" s="44"/>
       <c r="I18" s="29"/>
       <c r="J18" s="1"/>
       <c r="K18" s="29"/>
@@ -8866,14 +8868,14 @@
       <c r="A19" s="36" t="s">
         <v>1124</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="38" t="s">
         <v>1018</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="39" t="s">
         <v>1125</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="39" t="s">
+      <c r="D19" s="43"/>
+      <c r="E19" s="40" t="s">
         <v>1126</v>
       </c>
       <c r="F19" s="29"/>
@@ -8900,10 +8902,10 @@
       <c r="C20" s="30" t="s">
         <v>1128</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="37" t="s">
         <v>1129</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="37" t="s">
         <v>1130</v>
       </c>
       <c r="F20" s="29"/>
@@ -8927,7 +8929,7 @@
       <c r="B21" s="25" t="s">
         <v>1011</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="47" t="s">
         <v>1132</v>
       </c>
       <c r="E21" s="25" t="s">

</xml_diff>

<commit_message>
Add initial version of the new Stembureaus Open Data Standaard 1.4 version; Remove Leesloep as an example from the standaard and the invulformulier.
</commit_message>
<xml_diff>
--- a/files/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/files/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -29,7 +29,7 @@
   <si>
     <t xml:space="preserve">Op dit tabblad wordt het gebruik van deze spreadsheet toegelicht. Hieronder staat de beschrijving van de andere twee tabbladen 'Attributen' en 'Metadata'.
 Dit invulformulier is bedoeld om geüpload te worden naar https://waarismijnstemlokaal.nl/. In plaats van dit invulformulier kan ook de invultool op https://waarismijnstemlokaal.nl/ gebruikt worden. Ook kan op die website een versie van dit invulformulier gedownload worden waarin de stembureaus van de vorige verkiezing alvast (deels) ingevuld staan.
-Dit invulformulier is gebaseerd op de Stembureaus Open Data Standaard versie 1.3.</t>
+Dit invulformulier is gebaseerd op de Stembureaus Open Data Standaard versie 1.4.</t>
   </si>
   <si>
     <t xml:space="preserve">Attributen</t>
@@ -3220,10 +3220,10 @@
     <t xml:space="preserve">Visuele hulpmiddelen</t>
   </si>
   <si>
-    <t xml:space="preserve">Welke visuele hulpmiddelen zijn aanwezig? Dit is een vrij tekstveld.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">leesloep, stemmal, vrijwilliger/host aanwezig</t>
+    <t xml:space="preserve">Welke visuele hulpmiddelen zijn aanwezig? Dit is een vrij tekstveld. NB: een leesloep is verplicht op elk stembureau en moet hier dus niet vermeld worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stemmal, vrijwilliger/host aanwezig</t>
   </si>
   <si>
     <t xml:space="preserve">Gehandicaptentoilet</t>
@@ -4144,14 +4144,14 @@
     <cellStyle name="Heading 3" xfId="41"/>
     <cellStyle name="Heading 4" xfId="42"/>
     <cellStyle name="Heading 5" xfId="43"/>
-    <cellStyle name="Heading1" xfId="44"/>
+    <cellStyle name="Heading 1" xfId="44"/>
     <cellStyle name="Hyperlink 10" xfId="45"/>
     <cellStyle name="Hyperlink 11" xfId="46"/>
     <cellStyle name="Neutral 13" xfId="47"/>
     <cellStyle name="Neutral 14" xfId="48"/>
     <cellStyle name="Note 8" xfId="49"/>
     <cellStyle name="Note 9" xfId="50"/>
-    <cellStyle name="Result" xfId="51"/>
+    <cellStyle name="Result 1" xfId="51"/>
     <cellStyle name="Result2" xfId="52"/>
     <cellStyle name="Status 11" xfId="53"/>
     <cellStyle name="Status 12" xfId="54"/>
@@ -4231,7 +4231,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4241,12 +4241,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="78.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="2" width="10.82"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="2" width="10.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="2" width="10.82"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="2" width="10.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4254,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4287,8 +4287,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4297,7 +4297,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
@@ -4311,17 +4311,17 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="51.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="53.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="64.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="46.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="51.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="51.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1005" min="9" style="4" width="51.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1006" style="4" width="11.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="46.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="51.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="5" width="51.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1005" min="9" style="4" width="51.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1006" style="4" width="11.17"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8319,8 +8319,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8329,7 +8329,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8341,7 +8341,7 @@
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="19.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="17.66"/>
@@ -8349,7 +8349,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="25" width="79.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="25" width="69.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="25" width="75.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="25" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="25" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8939,7 +8939,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Update standard: Split Openingstijden into Openingstijd and Sluitingstijd; Add sheet with info about csv/json; allow mobiele stembureaus and those that are not in/close to a building to not fill in a BAG ID; make clear that stembureaus that are open during multiple days must use a different number; Add "Type stembureau"; add info about BAG ID cell format
</commit_message>
<xml_diff>
--- a/files/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/files/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -3066,58 +3066,6 @@
     <t xml:space="preserve">ja</t>
   </si>
   <si>
-    <t xml:space="preserve">Een stembureau is gevestigd in een stemlokaal en elk stembureau heeft een eigen nummer. Sommige stemlokalen hebben meerdere stembureaus. Elk stembureau moet apart ingevoerd worden ook al is de locatie (het stemlokaal) hetzelfde aangezien elk stembureau een ander nummer heeft.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cijfers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naam stembureau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tekst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stadhuis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website van de locatie van het stembureau, indien aanwezig; Een URL moet met 'http://' of 'https://' beginnen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.denhaag.nl/nl/bestuur-en-organisatie/contact-met-de-gemeente/stadhuis-den-haag.htm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG Nummeraanduiding ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG Nummeraanduiding ID, vindbaar door het adres van het stembureau op https://bagviewer.kadaster.nl/ in te voeren en rechts onder het kopje 'Nummeraanduiding' te kijken.
-Vermeld voor mobiele stembureaus of locaties zonder BAG Nummeraanduiding ID het dichtstbijzijnde BAG Nummeraanduiding ID en gebruik eventueel het 'Extra adresaanduiding'-veld om de locatie van stembureau te beschrijven. NB: de precieze locatie geeft u aan met de 'Latitude' en 'Longitude'-velden of met de ‘X’ en ‘Y’-velden.
-Caribisch Nederland (BES-eilanden) staat niet in de BAG. Deze gemeenten moeten '0000000000000000' (zestien keer het getal '0') invullen en het adres verplicht invullen in het 'Extra adresaanduiding'-attribuut.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0518200000747446</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extra adresaanduiding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja, als er '0000000000000000' is ingevuld bij 'BAG Nummeraanduiding ID'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eventuele extra informatie over de locatie van het stembureau. Bv. 'Ingang aan achterkant gebouw' of 'Mobiel stembureau op het midden van het plein'.
-Sommige stembureaus zijn niet open voor algemeen publiek vanwege coronamaatregelen. Bijvoorbeeld een stembureau in een verzorgingshuis. Geef dat in dit veld aan door exact de tekst 'Niet open voor algemeen publiek' in te voeren.
-Caribisch Nederland (BES-eilanden) vult verplicht hier het hele adres in.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -3126,7 +3074,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">tekst</t>
+      <t xml:space="preserve">Een stembureau is gevestigd in een stemlokaal en elk stembureau heeft een eigen nummer. Sommige stemlokalen hebben meerdere stembureaus. Elk stembureau moet apart ingevoerd worden ook al is de locatie (het stemlokaal) hetzelfde aangezien elk stembureau een ander nummer heeft.
+</t>
     </r>
     <r>
       <rPr>
@@ -3135,8 +3084,74 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">; als er geen extra informatie is, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
+      <t xml:space="preserve">
+Als een stembureau meerdere dagen open is dan hoort deze voor elke dag een ander stembureaunummer te hebben. Elke stembureau(nummer) moet dus apart ingevoerd worden.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">cijfers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naam stembureau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stadhuis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type stembureau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;type&gt;: keuze uit 'regulier', ‘bijzonder’ en ‘mobiel’.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;type&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website van de locatie van het stembureau, indien aanwezig; Een URL moet met 'http://' of 'https://' beginnen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.denhaag.nl/nl/bestuur-en-organisatie/contact-met-de-gemeente/stadhuis-den-haag.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG Nummeraanduiding ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG Nummeraanduiding ID, vindbaar door het adres van het stembureau op https://bagviewer.kadaster.nl/ in te voeren en rechts onder het kopje 'Nummeraanduiding' te kijken.
+Wordt de ID niet goed opgeslagen? Zorg dan dat de cel opgemaakt is als ‘tekst’ of plaats voor de ID één aanhalingsteken (').
+Vermeld voor mobiele stembureaus die vlakbij een gebouw staan of locaties zonder BAG Nummeraanduiding ID het BAG Nummeraanduiding ID van het dichtstbijzijnde gebouw en gebruik eventueel het 'Extra adresaanduiding'-veld om de locatie van stembureau te beschrijven. Mocht een (mobiel) stembureau niet in de buurt van een gebouw staan, voer dan '0000000000000000' (zestien keer het getal '0') in; 'Extra adresaanduiding'-attribuut is dan verplicht. NB: de precieze locatie geeft u aan met de 'Latitude' en 'Longitude'-velden.
+Caribisch Nederland (BES-eilanden) staat niet in de BAG. Deze gemeenten moeten '0000000000000000' (zestien keer het getal '0') invullen en het adres verplicht invullen in het 'Extra adresaanduiding'-attribuut.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0518200000747446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra adresaanduiding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja, als er '0000000000000000' is ingevuld bij 'BAG Nummeraanduiding ID'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventuele extra informatie over de locatie van het stembureau. Bv. 'Ingang aan achterkant gebouw' of 'Mobiel stembureau op het midden van het plein'.
+Sommige stembureaus zijn niet open voor algemeen publiek vanwege coronamaatregelen. Bijvoorbeeld een stembureau in een verzorgingshuis. Geef dat in dit veld aan door exact de tekst 'Niet open voor algemeen publiek' in te voeren.
+Caribisch Nederland (BES-eilanden) vult verplicht hier het hele adres in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst; als er geen extra informatie is, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
   </si>
   <si>
     <t xml:space="preserve">Ingang aan achterkant gebouw</t>
@@ -3181,34 +3196,22 @@
 Als u de longitude van het stembureau niet weet dan kunt u dit vinden via https://www.openstreetmap.org/. Zoom in op het stembureau, klik op de juiste locatie met de rechtermuisknop en selecteer 'Show address'/'Toon adres'. De latitude en longitude (in die volgorde) staan nu linksboven in de zoekbalk.</t>
   </si>
   <si>
-    <t xml:space="preserve">Openingstijden 14-03-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja, er minimaal één openingstijden-attribuut ingevuld worden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zie opmerking bij het ‘Openingstijden 16-03-2022’-attribuut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS tot YYYY-MM-DDTHH:MM:SS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-14T07:30:00 tot 2022-03-14T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 15-03-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-15T07:30:00 tot 2022-03-15T21:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openingstijden 16-03-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sommige gemeenten werken met mobiele stembureaus die gedurende de dag op verschillende locaties staan. Voor mobiele stembureaus moet elke locatie apart worden ingevoerd in een eigen 'Invulveld'-kolom (vul dus de hele kolom in en niet enkel de attributen die veranderen, zoals de locatie en openingstijden).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-16T07:30:00 tot 2022-03-16T21:00:00</t>
+    <t xml:space="preserve">Openingstijd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In sommige gevallen heeft een stembureau meerdere openingstijden, bijvoorbeeld een mobiel stemburea of een stembureau dat ‘s middags even dicht is. In zulke gevallen moeten voor alle openingstijden alle attributen apart ingevuld worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-16T07:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sluitingstijd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-16T21:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">Toegankelijk voor mensen met een lichamelijke beperking</t>
@@ -3228,25 +3231,7 @@
     <t xml:space="preserve">Is er een toegankelijke ov-halte in de buurt? Beschrijf hoe ver deze van het stembureau ligt en hoe deze toegankelijk is.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tekst</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">; als er geen toegankelijke ov-halte is, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
-    </r>
+    <t xml:space="preserve">tekst; als er geen toegankelijke ov-halte is, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
   </si>
   <si>
     <t xml:space="preserve">binnen 100 meter, rolstoeltoegankelijk, geleidelijnen</t>
@@ -3262,56 +3247,10 @@
     <t xml:space="preserve">Auditieve hulpmiddelen</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Welke auditieve hulpmiddelen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> voor slechthorende en doven</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> zijn aanwezig? Dit is een vrij tekstveld.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tekst; a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ls er geen hulpmiddelen zijn, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
-    </r>
+    <t xml:space="preserve">Welke auditieve hulpmiddelen voor slechthorende en doven zijn aanwezig? Dit is een vrij tekstveld.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst; als er geen hulpmiddelen zijn, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
   </si>
   <si>
     <t xml:space="preserve">gebarentolk, schrijftolk</t>
@@ -3320,56 +3259,10 @@
     <t xml:space="preserve">Visuele hulpmiddelen</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Welke visuele hulpmiddelen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> voor blinden en slechtzienden</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> zijn aanwezig? Dit is een vrij tekstveld.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tekst; a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ls er geen hulpmiddelen zijn, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd); NB: een leesloep is verplicht op elk stembureau en moet hier dus niet vermeld worden</t>
-    </r>
+    <t xml:space="preserve">Welke visuele hulpmiddelen voor blinden en slechtzienden zijn aanwezig? Dit is een vrij tekstveld.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst; als er geen hulpmiddelen zijn, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd); NB: een leesloep is verplicht op elk stembureau en moet hier dus niet vermeld worden</t>
   </si>
   <si>
     <t xml:space="preserve">stemmal, soundbox, vrijwilliger/host aanwezig, geleidelijnen</t>
@@ -3387,23 +3280,7 @@
     <t xml:space="preserve">Eventuele extra informatie over de toegankelijkheid van dit stembureau.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">prikkelarm stembureau, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">stembureau is volledig toegankelijk voor mensen met een lichamelijke beperking er is echter geen gehandicaptenparkeerplaats</t>
-    </r>
+    <t xml:space="preserve">prikkelarm stembureau, stembureau is volledig toegankelijk voor mensen met een lichamelijke beperking er is echter geen gehandicaptenparkeerplaats</t>
   </si>
   <si>
     <t xml:space="preserve">Tellocatie</t>
@@ -3639,7 +3516,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3806,22 +3683,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3969,7 +3841,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -4095,17 +3967,17 @@
     <xf numFmtId="164" fontId="21" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4178,6 +4050,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4198,8 +4074,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -4222,15 +4098,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7538,7 +7414,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="2" s="15" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="15" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>1010</v>
       </c>
@@ -7634,21 +7510,21 @@
       <c r="AMI3" s="4"/>
       <c r="AMJ3" s="4"/>
     </row>
-    <row r="4" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>1017</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1018</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>1019</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="12" t="s">
         <v>1020</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>1021</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="14"/>
@@ -7683,25 +7559,25 @@
       <c r="AMI4" s="4"/>
       <c r="AMJ4" s="4"/>
     </row>
-    <row r="5" s="15" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>1022</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>1011</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>1023</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>1013</v>
-      </c>
-      <c r="E5" s="13" t="s">
         <v>1024</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>1025</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="18"/>
+      <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
@@ -7732,25 +7608,25 @@
       <c r="AMI5" s="4"/>
       <c r="AMJ5" s="4"/>
     </row>
-    <row r="6" s="15" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="15" customFormat="true" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>1026</v>
-      </c>
-      <c r="C6" s="10" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>1027</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>1028</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>1029</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -7781,23 +7657,23 @@
       <c r="AMI6" s="4"/>
       <c r="AMJ6" s="4"/>
     </row>
-    <row r="7" s="15" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="15" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>1030</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>1031</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>1032</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="20" t="s">
         <v>1033</v>
       </c>
-      <c r="E7" s="17" t="n">
-        <v>81611</v>
-      </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -7835,16 +7711,16 @@
         <v>1034</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="E8" s="17" t="n">
-        <v>454909</v>
+        <v>81611</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="14"/>
@@ -7881,25 +7757,25 @@
     </row>
     <row r="9" s="15" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>1038</v>
-      </c>
-      <c r="D9" s="11" t="s">
         <v>1039</v>
       </c>
+      <c r="D9" s="10" t="s">
+        <v>1040</v>
+      </c>
       <c r="E9" s="17" t="n">
-        <v>52.0775912</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
+        <v>454909</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
@@ -7930,25 +7806,25 @@
     </row>
     <row r="10" s="15" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="E10" s="17" t="n">
-        <v>4.3166395</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+        <v>52.0775912</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
@@ -7977,21 +7853,21 @@
       <c r="AMI10" s="4"/>
       <c r="AMJ10" s="4"/>
     </row>
-    <row r="11" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="15" customFormat="true" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>1043</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>1044</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>1045</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>1046</v>
+      <c r="E11" s="17" t="n">
+        <v>4.3166395</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="14"/>
@@ -8027,20 +7903,20 @@
       <c r="AMJ11" s="4"/>
     </row>
     <row r="12" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="22" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>1047</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>1043</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1044</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>1045</v>
-      </c>
-      <c r="E12" s="13" t="s">
         <v>1048</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>1049</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="14"/>
@@ -8075,20 +7951,20 @@
       <c r="AMI12" s="4"/>
       <c r="AMJ12" s="4"/>
     </row>
-    <row r="13" s="15" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>1049</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>1043</v>
+    <row r="13" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>1011</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>1045</v>
-      </c>
-      <c r="E13" s="13" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E13" s="24" t="s">
         <v>1051</v>
       </c>
       <c r="F13" s="16"/>
@@ -8176,7 +8052,7 @@
         <v>1055</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>1056</v>
@@ -8223,7 +8099,7 @@
         <v>1059</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>1060</v>
@@ -8232,11 +8108,11 @@
         <v>1054</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="18"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -8272,7 +8148,7 @@
         <v>1061</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>1062</v>
@@ -8285,7 +8161,7 @@
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="18"/>
+      <c r="H17" s="19"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
@@ -8321,7 +8197,7 @@
         <v>1065</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>1066</v>
@@ -8334,7 +8210,7 @@
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="18"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
@@ -8370,7 +8246,7 @@
         <v>1069</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>1070</v>
@@ -8383,7 +8259,7 @@
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="18"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
@@ -8415,24 +8291,24 @@
       <c r="AMJ19" s="4"/>
     </row>
     <row r="20" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="22" t="s">
         <v>1071</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>1018</v>
+      <c r="B20" s="23" t="s">
+        <v>1022</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>1072</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>1028</v>
-      </c>
-      <c r="E20" s="23" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>1073</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="18"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
@@ -8468,7 +8344,7 @@
         <v>1074</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>1075</v>
@@ -8476,7 +8352,7 @@
       <c r="D21" s="10" t="s">
         <v>1054</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="25" t="s">
         <v>1011</v>
       </c>
       <c r="F21" s="16"/>
@@ -8513,7 +8389,7 @@
       <c r="AMJ21" s="4"/>
     </row>
     <row r="22" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="26" t="s">
         <v>1076</v>
       </c>
       <c r="B22" s="11" t="s">
@@ -8525,7 +8401,7 @@
       <c r="D22" s="11" t="s">
         <v>1078</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="27" t="s">
         <v>1079</v>
       </c>
       <c r="F22" s="16"/>
@@ -8562,7 +8438,7 @@
       <c r="AMJ22" s="4"/>
     </row>
     <row r="23" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="26" t="s">
         <v>1080</v>
       </c>
       <c r="B23" s="11" t="s">
@@ -8572,14 +8448,14 @@
         <v>1081</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>1020</v>
-      </c>
-      <c r="E23" s="26" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E23" s="27" t="s">
         <v>1082</v>
       </c>
-      <c r="F23" s="27"/>
+      <c r="F23" s="28"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="18"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
@@ -8636,73 +8512,73 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="28" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="28" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="28" width="70.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="28" width="79.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="28" width="69.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="28" width="75.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="28" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="70.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="29" width="79.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="29" width="69.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="29" width="75.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="29" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1083</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>1011</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="38" t="s">
         <v>1084</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="33" t="s">
         <v>1086</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="32"/>
+      <c r="I2" s="33"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
     </row>
     <row r="3" s="4" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>1087</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>1018</v>
+      <c r="B3" s="29" t="s">
+        <v>1022</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>1088</v>
@@ -8710,25 +8586,25 @@
       <c r="D3" s="11" t="s">
         <v>1089</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="29" t="s">
         <v>1090</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="40" t="s">
         <v>1091</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="35" t="s">
         <v>1011</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1092</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>1093</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="41" t="s">
         <v>1094</v>
       </c>
       <c r="F4" s="1"/>
@@ -8736,496 +8612,496 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="40" t="s">
         <v>1095</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="42" t="s">
         <v>1011</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="43" t="s">
         <v>1096</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="44" t="s">
         <v>1015</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="44" t="s">
         <v>1097</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>1098</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>1011</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="43" t="s">
         <v>1096</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="45" t="s">
         <v>1015</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="45" t="s">
         <v>1099</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="40" t="s">
         <v>1100</v>
       </c>
-      <c r="B7" s="41" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C7" s="42" t="s">
+      <c r="B7" s="42" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C7" s="43" t="s">
         <v>1096</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="45" t="s">
         <v>1015</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="45" t="s">
         <v>1101</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="40" t="s">
         <v>1102</v>
       </c>
-      <c r="B8" s="41" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C8" s="42" t="s">
+      <c r="B8" s="42" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>1096</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="45" t="s">
         <v>1015</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="45" t="s">
         <v>1103</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="40" t="s">
         <v>1104</v>
       </c>
-      <c r="B9" s="34" t="s">
-        <v>1018</v>
+      <c r="B9" s="35" t="s">
+        <v>1022</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1105</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="34" t="s">
         <v>1106</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="41" t="s">
         <v>1107</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="32"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="40" t="s">
         <v>1108</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="42" t="s">
         <v>1011</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="43" t="s">
         <v>1096</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44" t="s">
+      <c r="D10" s="45"/>
+      <c r="E10" s="45" t="s">
         <v>1109</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="40" t="s">
         <v>1110</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="42" t="s">
         <v>1011</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="43" t="s">
         <v>1096</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44" t="s">
+      <c r="D11" s="45"/>
+      <c r="E11" s="45" t="s">
         <v>1111</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="32"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="40" t="s">
         <v>1112</v>
       </c>
-      <c r="B12" s="34" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C12" s="33" t="s">
+      <c r="B12" s="35" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>1113</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="34" t="s">
         <v>1114</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="41" t="s">
         <v>1115</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="40" t="s">
         <v>1116</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>1011</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="34" t="s">
         <v>1117</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="34" t="s">
         <v>1118</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="46" t="s">
         <v>1119</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="40" t="s">
         <v>1120</v>
       </c>
-      <c r="B14" s="41" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C14" s="42" t="s">
+      <c r="B14" s="42" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C14" s="43" t="s">
         <v>1096</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46" t="s">
+      <c r="D14" s="47"/>
+      <c r="E14" s="47" t="s">
         <v>1121</v>
       </c>
-      <c r="F14" s="32"/>
+      <c r="F14" s="33"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="33"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="40" t="s">
         <v>1122</v>
       </c>
-      <c r="B15" s="34" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C15" s="33" t="s">
+      <c r="B15" s="35" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C15" s="34" t="s">
         <v>1123</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="34" t="s">
         <v>1124</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="19" t="s">
         <v>1125</v>
       </c>
-      <c r="F15" s="32"/>
+      <c r="F15" s="33"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="32"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="33"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="40" t="s">
         <v>1126</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="35" t="s">
         <v>1011</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="34" t="s">
         <v>1127</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="49" t="s">
         <v>1128</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="49" t="s">
         <v>1129</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="40" t="s">
         <v>1130</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="35" t="s">
         <v>1011</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="34" t="s">
         <v>1131</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="34" t="s">
         <v>1118</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="46" t="s">
         <v>1119</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="32"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="33"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="40" t="s">
         <v>1132</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="42" t="s">
         <v>1011</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="43" t="s">
         <v>1096</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49" t="s">
+      <c r="D18" s="50"/>
+      <c r="E18" s="50" t="s">
         <v>1133</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="32"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="40" t="s">
         <v>1134</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C19" s="42" t="s">
+      <c r="B19" s="42" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C19" s="43" t="s">
         <v>1135</v>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="43" t="s">
+      <c r="D19" s="47"/>
+      <c r="E19" s="44" t="s">
         <v>1136</v>
       </c>
-      <c r="F19" s="32"/>
+      <c r="F19" s="33"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="32"/>
+      <c r="I19" s="33"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="32"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="40" t="s">
         <v>1137</v>
       </c>
-      <c r="B20" s="34" t="s">
-        <v>1018</v>
-      </c>
-      <c r="C20" s="33" t="s">
+      <c r="B20" s="35" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>1138</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="41" t="s">
         <v>1139</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="41" t="s">
         <v>1140</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="39" t="s">
         <v>1141</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="29" t="s">
         <v>1011</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="C21" s="51" t="s">
         <v>1142</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="29" t="s">
         <v>1143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Stembureaus Open Data Standaard to version 1.5
</commit_message>
<xml_diff>
--- a/files/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/files/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -22,14 +22,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="1148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1144">
   <si>
     <t xml:space="preserve">Toelichting</t>
   </si>
   <si>
     <t xml:space="preserve">Op dit tabblad wordt het gebruik van deze spreadsheet toegelicht. Hieronder staat de beschrijving van de andere twee tabbladen 'Attributen' en 'Metadata'.
 Dit invulformulier is bedoeld om geüpload te worden naar https://waarismijnstemlokaal.nl/. In plaats van dit invulformulier kan ook de invultool op https://waarismijnstemlokaal.nl/ gebruikt worden. Ook kan op die website een versie van dit invulformulier gedownload worden waarin de stembureaus van de vorige verkiezing alvast (deels) ingevuld staan.
-Dit invulformulier is gebaseerd op de Stembureaus Open Data Standaard versie 1.4.</t>
+Dit invulformulier is gebaseerd op de Stembureaus Open Data Standaard versie 1.5.</t>
   </si>
   <si>
     <t xml:space="preserve">Attributen</t>
@@ -3185,13 +3185,13 @@
     <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-03-15T07:30:00</t>
+    <t xml:space="preserve">2023-11-22T07:30:00</t>
   </si>
   <si>
     <t xml:space="preserve">Sluitingstijd</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-03-15T21:00:00</t>
+    <t xml:space="preserve">2023-11-22T21:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">Toegankelijk voor mensen met een lichamelijke beperking</t>
@@ -3217,7 +3217,7 @@
     <t xml:space="preserve">binnen 100 meter, rolstoeltoegankelijk, geleidelijnen</t>
   </si>
   <si>
-    <t xml:space="preserve">Akoestiek</t>
+    <t xml:space="preserve">Akoestiek geschikt voor slechthorenden</t>
   </si>
   <si>
     <t xml:space="preserve">Is de akoestiek van het stembureau geschikt voor slechthorenden?
@@ -3290,21 +3290,6 @@
     <t xml:space="preserve">https://www.stembureausindenhaag.nl/</t>
   </si>
   <si>
-    <t xml:space="preserve">Verkiezingen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In het geval van waterschapsverkiezingen kan er in sommige gemeenten niet in elk stembureau voor elk waterschap gestemd worden. Door Amsterdam lopen er bijvoorbeeld drie waterschappen en er kan enkel voor een waterschap gestemd worden bij stembureaus die in het gebied van het waterschap liggen. Alle gemeenten vragen we daarom in het geval van deze verkiezingen per stembureau specifiek aan te geven voor welke waterschappen er gestemd kunnen worden. Ook als er überhaupt maar één keuze is (bv. als er in de hele gemeente maar voor één waterschap gekozen kan worden) en ook als er in de gemeente bij elk stembureau voor alle verkiezingen gestemd kan worden.
-In het geval dat er in dit stembureau voor meerdere waterschapen gestemd kan worden dan scheidt u deze met een puntkomma, bv.:
-Waterschapsverkiezingen voor Delfland; waterschapsverkiezingen voor Rijnland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keuze uit:
-– 'waterschapsverkiezingen voor &lt;naam van waterschap zonder "Waterschap" of "Hoogheemraadschap" voor de naam&gt;'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterschapsverkiezingen voor Delfland</t>
-  </si>
-  <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
@@ -3315,13 +3300,13 @@
     <t xml:space="preserve">Stembureaus &lt;verkiezing&gt; &lt;jaar&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Stembureaus Provinciale Statenverkiezingen 2023</t>
+    <t xml:space="preserve">Stembureaus Tweede Kamerverkiezingen 2023</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;CBS gemeentecode&gt;: code bestaande uit 6 karakters, zie https://opendata.cbs.nl/#/CBS/nl/dataset/85385NED/table?dl=B165 of gebruik GM9001 voor Bonaire, GM9002 voor Sint Eustatius of GM9003 voor Saba.
+    <t xml:space="preserve">&lt;CBS gemeentecode&gt;: code bestaande uit 6 karakters, zie https://opendata.cbs.nl/#/CBS/nl/dataset/70739ned/table?dl=5A68C of gebruik GM9001 voor Bonaire, GM9002 voor Sint Eustatius of GM9003 voor Saba.
 &lt;YYYYMMDD&gt;: datum van de verkiezing
 &lt;oplopend getal&gt;: getal tussen 000 en 999</t>
   </si>
@@ -3329,20 +3314,20 @@
     <t xml:space="preserve">NLODS&lt;CBS gemeentecode&gt;stembureaus&lt;YYYYMMDD&gt;&lt;oplopend getal van 000 t/m 999&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">NLODSGM0518stembureaus20230315010</t>
+    <t xml:space="preserve">NLODSGM0518stembureaus20231122014</t>
   </si>
   <si>
     <t xml:space="preserve">Omschrijving</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;verkiezing&gt;: keuze uit 'de Tweede Kamerverkiezingen', 'de gemeenteraadsverkiezingen', 'de Provinciale Statenverkiezingen', 'referendum &lt;naam van referendum&gt;', 'de kiescollegeverkiezingen', 'de eilandsraadsverkiezingen', 'de Europese Parlementsverkiezingen', 'de waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'
-&lt;datum&gt;: in format zoals '15 maart 2023'</t>
+&lt;datum&gt;: in format zoals '22 november 2023'</t>
   </si>
   <si>
     <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op &lt;verkiezing&gt; op &lt;datum&gt;.</t>
   </si>
   <si>
-    <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op de Provinciale Statenverkiezingen op 15 maart 2023.</t>
+    <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op de Tweede Kamerverkiezingen op 22 november 2023.</t>
   </si>
   <si>
     <t xml:space="preserve">Eigenaar</t>
@@ -3381,7 +3366,7 @@
     <t xml:space="preserve">verkiezingen, stembureaus, overheid, democratie, stemmen, kiesdistrict, &lt;aard van de verkiezing&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">verkiezingen, stembureaus, overheid, democratie, stemmen, kiesdistrict, gemeenteraadsverkiezingen</t>
+    <t xml:space="preserve">verkiezingen, stembureaus, overheid, democratie, stemmen, kiesdistrict, Tweede Kamerverkiezingen</t>
   </si>
   <si>
     <t xml:space="preserve">Thema</t>
@@ -3410,7 +3395,7 @@
     <t xml:space="preserve">&lt;gebied&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Europees Nederland</t>
+    <t xml:space="preserve">Nederland</t>
   </si>
   <si>
     <t xml:space="preserve">Datum publicatie</t>
@@ -3422,7 +3407,7 @@
     <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS+-HH:MM</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-01-16T13:05:23+01:00</t>
+    <t xml:space="preserve">2023-09-16T13:05:23+01:00</t>
   </si>
   <si>
     <t xml:space="preserve">Relatie / gebruik andere standaarden</t>
@@ -3440,19 +3425,19 @@
     <t xml:space="preserve">YYYY-MM-DD</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-03-15</t>
+    <t xml:space="preserve">2023-11-22</t>
   </si>
   <si>
     <t xml:space="preserve">Update frequentie</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;datum verkiezing&gt;: in format zoals '15 maart 2023'</t>
+    <t xml:space="preserve">&lt;datum verkiezing&gt;: in format zoals '22 november 2023'</t>
   </si>
   <si>
     <t xml:space="preserve">Incidenteel tot en met &lt;datum verkiezing&gt; (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezing)</t>
   </si>
   <si>
-    <t xml:space="preserve">Incidenteel tot en met 15 maart 2023 (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezingen)</t>
+    <t xml:space="preserve">Incidenteel tot en met 22 november 2023 (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezingen)</t>
   </si>
   <si>
     <t xml:space="preserve">Wijzigings datum</t>
@@ -3474,7 +3459,7 @@
 Invoer is "vast"</t>
   </si>
   <si>
-    <t xml:space="preserve">Stembureaus ODS 1.3</t>
+    <t xml:space="preserve">Stembureaus ODS 1.5</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -3511,7 +3496,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3705,6 +3690,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
@@ -3726,6 +3718,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3850,7 +3848,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -3979,14 +3977,14 @@
     <xf numFmtId="164" fontId="26" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4099,6 +4097,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4115,31 +4117,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4169,6 +4159,10 @@
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -4407,7 +4401,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ24"/>
+  <dimension ref="A1:AMJ23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -4419,7 +4413,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="24.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="53.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="64.17"/>
@@ -8128,7 +8122,7 @@
       <c r="AMJ15" s="6"/>
     </row>
     <row r="16" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="28" t="s">
         <v>1059</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -8385,7 +8379,7 @@
       <c r="D21" s="14" t="s">
         <v>1054</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="29" t="s">
         <v>1011</v>
       </c>
       <c r="F21" s="19"/>
@@ -8422,7 +8416,7 @@
       <c r="AMJ21" s="6"/>
     </row>
     <row r="22" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="30" t="s">
         <v>1076</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -8434,7 +8428,7 @@
       <c r="D22" s="15" t="s">
         <v>1078</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="31" t="s">
         <v>1079</v>
       </c>
       <c r="F22" s="19"/>
@@ -8471,7 +8465,7 @@
       <c r="AMJ22" s="6"/>
     </row>
     <row r="23" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="30" t="s">
         <v>1080</v>
       </c>
       <c r="B23" s="15" t="s">
@@ -8483,10 +8477,10 @@
       <c r="D23" s="15" t="s">
         <v>1024</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="31" t="s">
         <v>1082</v>
       </c>
-      <c r="F23" s="31"/>
+      <c r="F23" s="32"/>
       <c r="G23" s="18"/>
       <c r="H23" s="22"/>
       <c r="I23" s="18"/>
@@ -8519,36 +8513,6 @@
       <c r="AMI23" s="6"/>
       <c r="AMJ23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="25" t="s">
-        <v>1083</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>1022</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>1086</v>
-      </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8568,607 +8532,610 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="35" width="70.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="79.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="69.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="35" width="75.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="35" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="70.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="79.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="33" width="69.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="75.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="33" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="39"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42" t="s">
-        <v>1087</v>
-      </c>
-      <c r="B2" s="43" t="s">
+      <c r="A2" s="40" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>1011</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>1088</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>1090</v>
-      </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="C2" s="42" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="39"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="20"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B3" s="35" t="s">
+      <c r="A3" s="43" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>1022</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>1092</v>
+      <c r="C3" s="44" t="s">
+        <v>1088</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>1093</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>1094</v>
+        <v>1089</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>1090</v>
       </c>
       <c r="H3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="46" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="45" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>1011</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>1098</v>
+        <v>1092</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>1094</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="46" t="s">
-        <v>1099</v>
-      </c>
-      <c r="B5" s="48" t="s">
+      <c r="A5" s="45" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B5" s="47" t="s">
         <v>1011</v>
       </c>
-      <c r="C5" s="49" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D5" s="50" t="s">
+      <c r="C5" s="48" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D5" s="49" t="s">
         <v>1015</v>
       </c>
-      <c r="E5" s="50" t="s">
-        <v>1101</v>
+      <c r="E5" s="49" t="s">
+        <v>1097</v>
       </c>
       <c r="F5" s="20"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46" t="s">
-        <v>1102</v>
-      </c>
-      <c r="B6" s="48" t="s">
+      <c r="A6" s="45" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>1011</v>
       </c>
-      <c r="C6" s="49" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D6" s="51" t="s">
+      <c r="C6" s="48" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D6" s="50" t="s">
         <v>1015</v>
       </c>
-      <c r="E6" s="51" t="s">
-        <v>1103</v>
-      </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="E6" s="50" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="46" t="s">
-        <v>1104</v>
-      </c>
-      <c r="B7" s="48" t="s">
+      <c r="A7" s="45" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B7" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D7" s="51" t="s">
+      <c r="C7" s="48" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D7" s="50" t="s">
         <v>1015</v>
       </c>
-      <c r="E7" s="51" t="s">
-        <v>1105</v>
-      </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="E7" s="50" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="20"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="46" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B8" s="48" t="s">
+      <c r="A8" s="45" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B8" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="C8" s="49" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D8" s="51" t="s">
+      <c r="C8" s="48" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D8" s="50" t="s">
         <v>1015</v>
       </c>
-      <c r="E8" s="51" t="s">
-        <v>1107</v>
-      </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="E8" s="50" t="s">
+        <v>1103</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
     </row>
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="46" t="s">
-        <v>1108</v>
-      </c>
-      <c r="B9" s="41" t="s">
+      <c r="A9" s="45" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B9" s="39" t="s">
         <v>1022</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>1109</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>1110</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>1111</v>
+        <v>1105</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>1107</v>
       </c>
       <c r="F9" s="20"/>
-      <c r="G9" s="39"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="46" t="s">
-        <v>1112</v>
-      </c>
-      <c r="B10" s="48" t="s">
+      <c r="A10" s="45" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B10" s="47" t="s">
         <v>1011</v>
       </c>
-      <c r="C10" s="49" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51" t="s">
-        <v>1113</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
+      <c r="C10" s="48" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="46" t="s">
-        <v>1114</v>
-      </c>
-      <c r="B11" s="48" t="s">
+      <c r="A11" s="45" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B11" s="47" t="s">
         <v>1011</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51" t="s">
-        <v>1115</v>
-      </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="39"/>
+      <c r="C11" s="48" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F11" s="42"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="46" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B12" s="41" t="s">
+      <c r="A12" s="45" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B12" s="39" t="s">
         <v>1022</v>
       </c>
-      <c r="C12" s="40" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E12" s="47" t="s">
-        <v>1119</v>
+      <c r="C12" s="38" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>1115</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="20"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="39"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="46" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B13" s="41" t="s">
+      <c r="A13" s="45" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B13" s="39" t="s">
         <v>1011</v>
       </c>
-      <c r="C13" s="40" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>1122</v>
-      </c>
-      <c r="E13" s="52" t="s">
-        <v>1123</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="C13" s="38" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="20"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="46" t="s">
-        <v>1124</v>
-      </c>
-      <c r="B14" s="48" t="s">
+      <c r="A14" s="45" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B14" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="C14" s="49" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53" t="s">
-        <v>1125</v>
-      </c>
-      <c r="F14" s="39"/>
+      <c r="C14" s="48" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F14" s="37"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="46" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B15" s="41" t="s">
+      <c r="A15" s="45" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B15" s="39" t="s">
         <v>1022</v>
       </c>
-      <c r="C15" s="40" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>1128</v>
+      <c r="C15" s="38" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>1124</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>1129</v>
-      </c>
-      <c r="F15" s="39"/>
+        <v>1125</v>
+      </c>
+      <c r="F15" s="37"/>
       <c r="G15" s="20"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="39"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="20"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="39"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="46" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B16" s="41" t="s">
+      <c r="A16" s="45" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B16" s="39" t="s">
         <v>1011</v>
       </c>
-      <c r="C16" s="40" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D16" s="55" t="s">
-        <v>1132</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>1133</v>
-      </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="39"/>
+      <c r="C16" s="38" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="46" t="s">
-        <v>1134</v>
-      </c>
-      <c r="B17" s="41" t="s">
+      <c r="A17" s="45" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B17" s="39" t="s">
         <v>1011</v>
       </c>
-      <c r="C17" s="40" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>1122</v>
-      </c>
-      <c r="E17" s="52" t="s">
-        <v>1123</v>
-      </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="39"/>
+      <c r="C17" s="38" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>1119</v>
+      </c>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="37"/>
       <c r="J17" s="20"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="46" t="s">
-        <v>1136</v>
-      </c>
-      <c r="B18" s="48" t="s">
+      <c r="A18" s="45" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B18" s="47" t="s">
         <v>1011</v>
       </c>
-      <c r="C18" s="49" t="s">
-        <v>1100</v>
-      </c>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="39"/>
+      <c r="C18" s="48" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F18" s="42"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="20"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="39"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="46" t="s">
-        <v>1138</v>
-      </c>
-      <c r="B19" s="48" t="s">
+      <c r="A19" s="45" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B19" s="47" t="s">
         <v>1022</v>
       </c>
-      <c r="C19" s="49" t="s">
-        <v>1139</v>
-      </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="50" t="s">
-        <v>1140</v>
-      </c>
-      <c r="F19" s="39"/>
+      <c r="C19" s="48" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D19" s="52"/>
+      <c r="E19" s="49" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F19" s="37"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="39"/>
+      <c r="I19" s="37"/>
       <c r="J19" s="20"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="46" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B20" s="41" t="s">
+      <c r="A20" s="45" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B20" s="39" t="s">
         <v>1022</v>
       </c>
-      <c r="C20" s="40" t="s">
-        <v>1142</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E20" s="47" t="s">
-        <v>1144</v>
-      </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
+      <c r="C20" s="38" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
       <c r="J20" s="20"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="45" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B21" s="35" t="s">
+      <c r="A21" s="43" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B21" s="33" t="s">
         <v>1011</v>
       </c>
-      <c r="C21" s="57" t="s">
-        <v>1146</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>1147</v>
+      <c r="C21" s="56" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>1143</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" location="/CBS/nl/dataset/70739ned/table?dl=5A68C" display="https://opendata.cbs.nl/#/CBS/nl/dataset/70739ned/table?dl=5A68C"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Big update for 2023TK elections; remove hardcoded dates; small fixes, also relating to previous change dynamically detect the "Verkiezingen" attribute
</commit_message>
<xml_diff>
--- a/files/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/files/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -3496,7 +3496,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3690,13 +3690,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
@@ -3718,12 +3711,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3848,7 +3835,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -3977,14 +3964,14 @@
     <xf numFmtId="164" fontId="26" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4097,10 +4084,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4121,15 +4104,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4159,10 +4142,6 @@
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -4413,7 +4392,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="53.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="64.17"/>
@@ -8122,7 +8101,7 @@
       <c r="AMJ15" s="6"/>
     </row>
     <row r="16" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="25" t="s">
         <v>1059</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -8379,7 +8358,7 @@
       <c r="D21" s="14" t="s">
         <v>1054</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="28" t="s">
         <v>1011</v>
       </c>
       <c r="F21" s="19"/>
@@ -8416,7 +8395,7 @@
       <c r="AMJ21" s="6"/>
     </row>
     <row r="22" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="29" t="s">
         <v>1076</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -8428,7 +8407,7 @@
       <c r="D22" s="15" t="s">
         <v>1078</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="30" t="s">
         <v>1079</v>
       </c>
       <c r="F22" s="19"/>
@@ -8465,7 +8444,7 @@
       <c r="AMJ22" s="6"/>
     </row>
     <row r="23" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="29" t="s">
         <v>1080</v>
       </c>
       <c r="B23" s="15" t="s">
@@ -8477,10 +8456,10 @@
       <c r="D23" s="15" t="s">
         <v>1024</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="30" t="s">
         <v>1082</v>
       </c>
-      <c r="F23" s="32"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="18"/>
       <c r="H23" s="22"/>
       <c r="I23" s="18"/>
@@ -8539,99 +8518,99 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="70.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="79.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="33" width="69.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="75.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="33" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="32" width="70.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="32" width="79.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="32" width="69.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="32" width="75.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="32" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="37"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>1083</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>1011</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="41" t="s">
         <v>1084</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="41" t="s">
         <v>1085</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="36" t="s">
         <v>1086</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="37"/>
+      <c r="I2" s="36"/>
       <c r="J2" s="20"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>1087</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>1022</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="15" t="s">
         <v>1088</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>1089</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>1090</v>
       </c>
       <c r="H3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>1091</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
         <v>1011</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>1092</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="37" t="s">
         <v>1093</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="44" t="s">
         <v>1094</v>
       </c>
       <c r="F4" s="20"/>
@@ -8639,502 +8618,502 @@
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>1095</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="45" t="s">
         <v>1011</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="46" t="s">
         <v>1096</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="47" t="s">
         <v>1015</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="47" t="s">
         <v>1097</v>
       </c>
       <c r="F5" s="20"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
         <v>1098</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="45" t="s">
         <v>1011</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="46" t="s">
         <v>1096</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="48" t="s">
         <v>1015</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="48" t="s">
         <v>1099</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="43" t="s">
         <v>1100</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="45" t="s">
         <v>1022</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="46" t="s">
         <v>1096</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="48" t="s">
         <v>1015</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="48" t="s">
         <v>1101</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="20"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="43" t="s">
         <v>1102</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="45" t="s">
         <v>1022</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="46" t="s">
         <v>1096</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="48" t="s">
         <v>1015</v>
       </c>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="48" t="s">
         <v>1103</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
     </row>
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>1104</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="38" t="s">
         <v>1022</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>1105</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="37" t="s">
         <v>1106</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="44" t="s">
         <v>1107</v>
       </c>
       <c r="F9" s="20"/>
-      <c r="G9" s="37"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="43" t="s">
         <v>1108</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="45" t="s">
         <v>1011</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="46" t="s">
         <v>1096</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50" t="s">
+      <c r="D10" s="48"/>
+      <c r="E10" s="48" t="s">
         <v>1109</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="43" t="s">
         <v>1110</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="45" t="s">
         <v>1011</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="46" t="s">
         <v>1096</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50" t="s">
+      <c r="D11" s="48"/>
+      <c r="E11" s="48" t="s">
         <v>1111</v>
       </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="37"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="43" t="s">
         <v>1112</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="38" t="s">
         <v>1022</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="37" t="s">
         <v>1113</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="37" t="s">
         <v>1114</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="44" t="s">
         <v>1115</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="20"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="43" t="s">
         <v>1116</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="37" t="s">
         <v>1117</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="37" t="s">
         <v>1118</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="49" t="s">
         <v>1119</v>
       </c>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="20"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="43" t="s">
         <v>1120</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="45" t="s">
         <v>1022</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="46" t="s">
         <v>1096</v>
       </c>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52" t="s">
+      <c r="D14" s="50"/>
+      <c r="E14" s="50" t="s">
         <v>1121</v>
       </c>
-      <c r="F14" s="37"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>1122</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="38" t="s">
         <v>1022</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="37" t="s">
         <v>1123</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="37" t="s">
         <v>1124</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>1125</v>
       </c>
-      <c r="F15" s="37"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="20"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="37"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="20"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="43" t="s">
         <v>1126</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="37" t="s">
         <v>1127</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="52" t="s">
         <v>1128</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="52" t="s">
         <v>1129</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="37"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="43" t="s">
         <v>1130</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="37" t="s">
         <v>1131</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="37" t="s">
         <v>1118</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="49" t="s">
         <v>1119</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="37"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="36"/>
       <c r="J17" s="20"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="43" t="s">
         <v>1132</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="45" t="s">
         <v>1011</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="46" t="s">
         <v>1096</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55" t="s">
+      <c r="D18" s="53"/>
+      <c r="E18" s="53" t="s">
         <v>1133</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="37"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="20"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="43" t="s">
         <v>1134</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="45" t="s">
         <v>1022</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="46" t="s">
         <v>1135</v>
       </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="49" t="s">
+      <c r="D19" s="50"/>
+      <c r="E19" s="47" t="s">
         <v>1136</v>
       </c>
-      <c r="F19" s="37"/>
+      <c r="F19" s="36"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="37"/>
+      <c r="I19" s="36"/>
       <c r="J19" s="20"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="43" t="s">
         <v>1137</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="38" t="s">
         <v>1022</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="37" t="s">
         <v>1138</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="44" t="s">
         <v>1139</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="44" t="s">
         <v>1140</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
       <c r="J20" s="20"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="42" t="s">
         <v>1141</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>1011</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="54" t="s">
         <v>1142</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="32" t="s">
         <v>1143</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" location="/CBS/nl/dataset/70739ned/table?dl=5A68C" display="https://opendata.cbs.nl/#/CBS/nl/dataset/70739ned/table?dl=5A68C"/>
+    <hyperlink ref="C3" r:id="rId1" location="/CBS/nl/dataset/70739ned/table?dl=5A68C" display="&lt;CBS gemeentecode&gt;: code bestaande uit 6 karakters, zie https://opendata.cbs.nl/#/CBS/nl/dataset/70739ned/table?dl=5A68C of gebruik GM9001 voor Bonaire, GM9002 voor Sint Eustatius of GM9003 voor Saba.&#10;&#10;&lt;YYYYMMDD&gt;: datum van de verkiezing&#10;&#10;&lt;oplopend getal&gt;: getal tussen 000 en 999"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Big update for 2024EP, part 1; Update Stembureaus Open Data Standaard to version 1.6
</commit_message>
<xml_diff>
--- a/files/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/files/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -22,14 +22,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="1157">
   <si>
     <t xml:space="preserve">Toelichting</t>
   </si>
   <si>
     <t xml:space="preserve">Op dit tabblad wordt het gebruik van deze spreadsheet toegelicht. Hieronder staat de beschrijving van de andere twee tabbladen 'Attributen' en 'Metadata'.
-Dit invulformulier is bedoeld om geüpload te worden naar https://waarismijnstemlokaal.nl/. In plaats van dit invulformulier kan ook de invultool op https://waarismijnstemlokaal.nl/ gebruikt worden. Ook kan op die website een versie van dit invulformulier gedownload worden waarin de stembureaus van de vorige verkiezing alvast (deels) ingevuld staan.
-Dit invulformulier is gebaseerd op de Stembureaus Open Data Standaard versie 1.5.</t>
+Dit invulformulier is bedoeld om geüpload te worden naar https://WaarIsMijnStemlokaal.nl/. In plaats van dit invulformulier kan ook de invultool op https://WaarIsMijnStemlokaal.nl/ gebruikt worden. Ook kan op die website een versie van dit invulformulier gedownload worden waarin de stembureaus van de vorige verkiezing alvast (deels) ingevuld staan.
+Dit invulformulier is gebaseerd op de Stembureaus Open Data Standaard versie 1.6.</t>
   </si>
   <si>
     <t xml:space="preserve">Attributen</t>
@@ -39,7 +39,7 @@
 Elk stembureau voegt u toe in een eigen 'Invulveld'-kolom waar u minimaal alle verplichte attributen (aangegeven met 'ja') invult (NB: in sommige gevallen kan hiervan worden afgeweken zoals beschreven in de opmerkingen bij een attribuut).
 De kolommen 'Opmerkingen, 'Format' en 'Voorbeeld' helpen u daarbij. De 'Opmerkingen'-kolom geeft algemene informatie over het attribuut en geeft soms meer informatie over hoe u het veld moet invullen zoals gespecificeerd in de 'Format'-kolom. In de 'Voorbeeld'-kolom wordt een voorbeeld gegeven van hoe u het attribuut moet invullen.
 Sommige gemeenten werken met mobiele stembureaus die gedurende de dag op verschillende locaties staan. Voor mobiele stembureaus moet elke locatie apart worden ingevoerd in een eigen 'Invulveld'-kolom (vul dus hele kolom in en niet enkel de attributen die veranderen, zoals de locatie en openingstijden).
-Er zijn 1000 'Invulveld'-kolommen, aangezien de gemeente met de meeste stembureaus (Amsterdam) er bijna 500 heeft en er voor mobiele stembureaus dus meerdere 'Invulveld'-kolommen nodig zijn. Mocht dit toch niet genoeg zijn dan kunt u gewoon extra kolommen aanmaken en ze doornummeren.</t>
+Er zijn 1000 'Invulveld'-kolommen, aangezien de gemeente met de meeste stembureaus (Amsterdam) er circa 500 heeft en er voor mobiele stembureaus dus meerdere 'Invulveld'-kolommen nodig zijn. Mocht dit toch niet genoeg zijn dan kunt u gewoon extra kolommen aanmaken en ze doornummeren.</t>
   </si>
   <si>
     <t xml:space="preserve">Metadata</t>
@@ -3106,7 +3106,7 @@
     <t xml:space="preserve">URL</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.denhaag.nl/nl/bestuur-en-organisatie/contact-met-de-gemeente/stadhuis-den-haag.htm</t>
+    <t xml:space="preserve">https://www.denhaag.nl/nl/contact-met-de-gemeente/stadhuis-den-haag/</t>
   </si>
   <si>
     <t xml:space="preserve">BAG Nummeraanduiding ID</t>
@@ -3185,21 +3185,19 @@
     <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-11-22T07:30:00</t>
+    <t xml:space="preserve">2024-06-06T07:30:00</t>
   </si>
   <si>
     <t xml:space="preserve">Sluitingstijd</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-11-22T21:00:00</t>
+    <t xml:space="preserve">2024-06-06T21:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">Toegankelijk voor mensen met een lichamelijke beperking</t>
   </si>
   <si>
-    <t xml:space="preserve">Is het stembureau toegankelijk voor mensen met een lichamelijke beperking?
-Voor meer informatie, zie:
-https://www.rijksoverheid.nl/onderwerpen/verkiezingen/verkiezingentoolkit/toegankelijkheid-verkiezingen</t>
+    <t xml:space="preserve">Is het stembureau toegankelijk voor mensen met een lichamelijke beperking? Voor meer informatie, zie: https://www.rijksoverheid.nl/onderwerpen/verkiezingen/verkiezingentoolkit/toegankelijkheid-verkiezingen.</t>
   </si>
   <si>
     <t xml:space="preserve">ja of nee</t>
@@ -3208,59 +3206,115 @@
     <t xml:space="preserve">Toegankelijke ov-halte</t>
   </si>
   <si>
-    <t xml:space="preserve">Is er een toegankelijke ov-halte in de buurt? Beschrijf hoe ver deze van het stembureau ligt en hoe deze toegankelijk is.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tekst; als er geen toegankelijke ov-halte is, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">binnen 100 meter, rolstoeltoegankelijk, geleidelijnen</t>
+    <t xml:space="preserve">Is er een toegankelijke ov-halte in de buurt?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gehandicaptentoilet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is er een gehandicaptentoilet aanwezig? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is er iemand aanwezig die kiezers ontvangt en kan helpen?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geleidelijnen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zijn er geleidelijnen aanwezig buiten en/of binnen het stembureau voor mensen met een visuele beperking?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keuze uit: 'buiten en binnen', 'buiten', 'binnen', 'nee'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buiten en binnen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stemmal met audio-ondersteuning</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Is er een stemmal met audio-ondersteuning (stembox/soundbox) aanwezig voor mensen met een visuele beperking of mensen die moeite hebben met lezen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">? Voor meer informatie, zie: https://www.oogvereniging.nl/leven-met/stemmen-met-een-oogaandoening/#stemmal, https://stemmal.nl/ en https://www.stembox.nl/.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Kandidatenlijst in braille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is er een kandidatenlijst in braille aanwezig voor mensen met een visuele beperking?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kandidatenlijst met grote letters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is er een kandidatenlijst met grote letters aanwezig voor mensen met een visuele beperking?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gebarentolk (NGT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is er een gebarentolk op locatie in het stembureau of op afstand (via videobellen) aanwezig die de Nederlandse Gebarentaal (NGT) beheerst? Als de gebarentolk niet de hele dag aanwezig is, vermeldt dan gedurende welke periode(n) deze precies aanwezig is in het 'Extra toegankelijkheidsinformatie'-attribuut.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keuze uit: 'op locatie', 'op afstand', 'nee'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">op locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gebarentalig stembureaulid (NGT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is er een stembureaulid aanwezig die de Nederlandse Gebarentaal (NGT) beheerst?</t>
   </si>
   <si>
     <t xml:space="preserve">Akoestiek geschikt voor slechthorenden</t>
   </si>
   <si>
-    <t xml:space="preserve">Is de akoestiek van het stembureau geschikt voor slechthorenden?
-Voor meer informatie, zie: https://bk.nijsnet.com/04040_Slechthorenden.aspx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auditieve hulpmiddelen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welke auditieve hulpmiddelen voor slechthorende en doven zijn aanwezig? Dit is een vrij tekstveld.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tekst; als er geen hulpmiddelen zijn, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gebarentolk, schrijftolk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visuele hulpmiddelen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welke visuele hulpmiddelen voor blinden en slechtzienden zijn aanwezig? Dit is een vrij tekstveld.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tekst; als er geen hulpmiddelen zijn, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd); NB: een leesloep is verplicht op elk stembureau en moet hier dus niet vermeld worden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stemmal, soundbox, vrijwilliger/host aanwezig, geleidelijnen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gehandicaptentoilet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is er een gehandicaptentoilet aanwezig? </t>
+    <t xml:space="preserve">Is de akoestiek van het stembureau geschikt voor slechthorenden? Voor meer informatie, zie: https://bk.nijsnet.nl/d_ontwerpregels/40_Slechthorenden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prikkelarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dit stembureau is zo ingericht dat er weinig prikkels zijn.</t>
   </si>
   <si>
     <t xml:space="preserve">Extra toegankelijkheidsinformatie</t>
   </si>
   <si>
-    <t xml:space="preserve">Eventuele extra informatie over de toegankelijkheid van dit stembureau.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prikkelarm stembureau, stembureau is volledig toegankelijk voor mensen met een lichamelijke beperking er is echter geen gehandicaptenparkeerplaats</t>
+    <t xml:space="preserve">Eventuele extra informatie over de toegankelijkheid van dit stembureau. Zie ook de voorbeelden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tekst; als er geen extra informatie is, laat dit veld dan leeg (‘nee’ e.d. worden automatisch verwijderd). NB: een leesloep is verplicht op elk stembureau en moet hier dus niet vermeld worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dit stembureau is ingericht voor kwetsbare mensen, stembureau is volledig toegankelijk voor mensen met een lichamelijke beperking er is echter geen gehandicaptenparkeerplaats, gebarentolk op locatie (NGT) is aanwezig van 10:00-12:00 en 16:00-18:00, oefenstembureau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overige informatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventuele overige informatie over dit stembureau.</t>
   </si>
   <si>
     <t xml:space="preserve">Tellocatie</t>
@@ -3300,7 +3354,7 @@
     <t xml:space="preserve">Stembureaus &lt;verkiezing&gt; &lt;jaar&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Stembureaus Tweede Kamerverkiezingen 2023</t>
+    <t xml:space="preserve">Stembureaus Europese Parlementsverkiezingen 2024</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -3314,20 +3368,20 @@
     <t xml:space="preserve">NLODS&lt;CBS gemeentecode&gt;stembureaus&lt;YYYYMMDD&gt;&lt;oplopend getal van 000 t/m 999&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">NLODSGM0518stembureaus20231122014</t>
+    <t xml:space="preserve">NLODSGM0518stembureaus20240606015</t>
   </si>
   <si>
     <t xml:space="preserve">Omschrijving</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;verkiezing&gt;: keuze uit 'de Tweede Kamerverkiezingen', 'de gemeenteraadsverkiezingen', 'de Provinciale Statenverkiezingen', 'referendum &lt;naam van referendum&gt;', 'de kiescollegeverkiezingen', 'de eilandsraadsverkiezingen', 'de Europese Parlementsverkiezingen', 'de waterschapsverkiezingen', 'verkiezingen gebiedscommissies en wijkraden' en 'verkiezingen stadsdeelcommissies'
-&lt;datum&gt;: in format zoals '22 november 2023'</t>
+&lt;datum&gt;: in format zoals '6 juni 2024'</t>
   </si>
   <si>
     <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op &lt;verkiezing&gt; op &lt;datum&gt;.</t>
   </si>
   <si>
-    <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op de Tweede Kamerverkiezingen op 22 november 2023.</t>
+    <t xml:space="preserve">Overzicht van de locaties van stembureaus. De gegevens hebben betrekking op de Europese Parlementsverkiezingen op 6 juni 2024.</t>
   </si>
   <si>
     <t xml:space="preserve">Eigenaar</t>
@@ -3366,7 +3420,7 @@
     <t xml:space="preserve">verkiezingen, stembureaus, overheid, democratie, stemmen, kiesdistrict, &lt;aard van de verkiezing&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">verkiezingen, stembureaus, overheid, democratie, stemmen, kiesdistrict, Tweede Kamerverkiezingen</t>
+    <t xml:space="preserve">verkiezingen, stembureaus, overheid, democratie, stemmen, kiesdistrict, Europese Parlementsverkiezingen</t>
   </si>
   <si>
     <t xml:space="preserve">Thema</t>
@@ -3407,7 +3461,7 @@
     <t xml:space="preserve">YYYY-MM-DDTHH:MM:SS+-HH:MM</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-09-16T13:05:23+01:00</t>
+    <t xml:space="preserve">2024-04-15T13:05:23+01:00</t>
   </si>
   <si>
     <t xml:space="preserve">Relatie / gebruik andere standaarden</t>
@@ -3425,19 +3479,19 @@
     <t xml:space="preserve">YYYY-MM-DD</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-11-22</t>
+    <t xml:space="preserve">2024-06-06</t>
   </si>
   <si>
     <t xml:space="preserve">Update frequentie</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;datum verkiezing&gt;: in format zoals '22 november 2023'</t>
+    <t xml:space="preserve">&lt;datum verkiezing&gt;: in format zoals '6 juni 2024'</t>
   </si>
   <si>
     <t xml:space="preserve">Incidenteel tot en met &lt;datum verkiezing&gt; (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezing)</t>
   </si>
   <si>
-    <t xml:space="preserve">Incidenteel tot en met 22 november 2023 (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezingen)</t>
+    <t xml:space="preserve">Incidenteel tot en met 6 juni 2024 (uiterste bekendmaking van stembureaus is 4 dagen voor de verkiezingen)</t>
   </si>
   <si>
     <t xml:space="preserve">Wijzigings datum</t>
@@ -3459,7 +3513,7 @@
 Invoer is "vast"</t>
   </si>
   <si>
-    <t xml:space="preserve">Stembureaus ODS 1.5</t>
+    <t xml:space="preserve">Stembureaus ODS 1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -3496,7 +3550,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3683,11 +3737,22 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3835,7 +3900,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -3961,17 +4026,17 @@
     <xf numFmtId="164" fontId="23" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="10" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="11" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4056,18 +4121,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="62" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4080,8 +4149,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -4096,23 +4177,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="63" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="12" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="30" fillId="12" borderId="0" xfId="64" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4380,7 +4457,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ23"/>
+  <dimension ref="A1:AMJ30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -7725,7 +7802,7 @@
       <c r="D8" s="14" t="s">
         <v>1037</v>
       </c>
-      <c r="E8" s="21" t="n">
+      <c r="E8" s="24" t="n">
         <v>81611</v>
       </c>
       <c r="F8" s="17"/>
@@ -7774,7 +7851,7 @@
       <c r="D9" s="14" t="s">
         <v>1040</v>
       </c>
-      <c r="E9" s="21" t="n">
+      <c r="E9" s="24" t="n">
         <v>454909</v>
       </c>
       <c r="F9" s="17"/>
@@ -7823,14 +7900,14 @@
       <c r="D10" s="15" t="s">
         <v>1043</v>
       </c>
-      <c r="E10" s="21" t="n">
+      <c r="E10" s="24" t="n">
         <v>52.0775912</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
@@ -7872,7 +7949,7 @@
       <c r="D11" s="15" t="s">
         <v>1043</v>
       </c>
-      <c r="E11" s="21" t="n">
+      <c r="E11" s="24" t="n">
         <v>4.3166395</v>
       </c>
       <c r="F11" s="19"/>
@@ -7909,10 +7986,10 @@
       <c r="AMJ11" s="6"/>
     </row>
     <row r="12" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>1046</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="27" t="s">
         <v>1011</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -7921,7 +7998,7 @@
       <c r="D12" s="14" t="s">
         <v>1048</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="28" t="s">
         <v>1049</v>
       </c>
       <c r="F12" s="19"/>
@@ -7958,10 +8035,10 @@
       <c r="AMJ12" s="6"/>
     </row>
     <row r="13" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="26" t="s">
         <v>1050</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="27" t="s">
         <v>1011</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -7970,7 +8047,7 @@
       <c r="D13" s="14" t="s">
         <v>1048</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="28" t="s">
         <v>1051</v>
       </c>
       <c r="F13" s="19"/>
@@ -8019,7 +8096,7 @@
       <c r="D14" s="14" t="s">
         <v>1054</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="24" t="s">
         <v>1011</v>
       </c>
       <c r="H14" s="18"/>
@@ -8053,7 +8130,7 @@
       <c r="AMI14" s="6"/>
       <c r="AMJ14" s="6"/>
     </row>
-    <row r="15" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
         <v>1055</v>
       </c>
@@ -8064,10 +8141,10 @@
         <v>1056</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>1057</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>1058</v>
+        <v>1054</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>1011</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
@@ -8100,21 +8177,21 @@
       <c r="AMI15" s="6"/>
       <c r="AMJ15" s="6"/>
     </row>
-    <row r="16" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25" t="s">
-        <v>1059</v>
+    <row r="16" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="s">
+        <v>1057</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>1022</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>1060</v>
+      <c r="C16" s="15" t="s">
+        <v>1058</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>1054</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>1022</v>
+      <c r="E16" s="24" t="s">
+        <v>1011</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="18"/>
@@ -8149,21 +8226,21 @@
       <c r="AMI16" s="6"/>
       <c r="AMJ16" s="6"/>
     </row>
-    <row r="17" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>1022</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>1062</v>
+      <c r="C17" s="15" t="s">
+        <v>1060</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>1063</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>1064</v>
+        <v>1054</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>1011</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="18"/>
@@ -8200,19 +8277,19 @@
     </row>
     <row r="18" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>1022</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>1067</v>
+      <c r="C18" s="29" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>1063</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="18"/>
@@ -8247,20 +8324,20 @@
       <c r="AMI18" s="6"/>
       <c r="AMJ18" s="6"/>
     </row>
-    <row r="19" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>1022</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>1070</v>
+      <c r="C19" s="29" t="s">
+        <v>1066</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>1054</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="24" t="s">
         <v>1011</v>
       </c>
       <c r="F19" s="18"/>
@@ -8296,21 +8373,21 @@
       <c r="AMI19" s="6"/>
       <c r="AMJ19" s="6"/>
     </row>
-    <row r="20" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="25" t="s">
-        <v>1071</v>
-      </c>
-      <c r="B20" s="26" t="s">
+    <row r="20" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>1022</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>1072</v>
+      <c r="C20" s="15" t="s">
+        <v>1068</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>1032</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>1073</v>
+        <v>1054</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>1011</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -8345,20 +8422,20 @@
       <c r="AMI20" s="6"/>
       <c r="AMJ20" s="6"/>
     </row>
-    <row r="21" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>1074</v>
+        <v>1069</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>1022</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>1075</v>
+        <v>1070</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>1054</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="24" t="s">
         <v>1011</v>
       </c>
       <c r="F21" s="19"/>
@@ -8394,21 +8471,21 @@
       <c r="AMI21" s="6"/>
       <c r="AMJ21" s="6"/>
     </row>
-    <row r="22" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="29" t="s">
-        <v>1076</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>1011</v>
+    <row r="22" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>1022</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>1079</v>
+        <v>1072</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>1074</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="18"/>
@@ -8444,20 +8521,20 @@
       <c r="AMJ22" s="6"/>
     </row>
     <row r="23" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="29" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="13" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E23" s="24" t="s">
         <v>1011</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>1081</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>1024</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>1082</v>
       </c>
       <c r="F23" s="31"/>
       <c r="G23" s="18"/>
@@ -8492,6 +8569,123 @@
       <c r="AMI23" s="6"/>
       <c r="AMJ23" s="6"/>
     </row>
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E27" s="24"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="33" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="33" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>1095</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8518,603 +8712,600 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="32" width="19.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="32" width="70.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="32" width="79.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="32" width="69.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="32" width="75.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="32" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="19.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="35" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="35" width="70.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="79.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="69.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="35" width="75.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="35" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="36"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>1083</v>
-      </c>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="42" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>1011</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>1086</v>
-      </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="C2" s="44" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="36"/>
+      <c r="I2" s="39"/>
       <c r="J2" s="20"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
-        <v>1087</v>
-      </c>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="45" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>1022</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>1088</v>
+      <c r="C3" s="29" t="s">
+        <v>1101</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>1090</v>
+        <v>1102</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>1103</v>
       </c>
       <c r="H3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="43" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B4" s="38" t="s">
+      <c r="A4" s="46" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>1011</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>1092</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>1093</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>1094</v>
+        <v>1105</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>1107</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B5" s="45" t="s">
+      <c r="A5" s="46" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B5" s="48" t="s">
         <v>1011</v>
       </c>
-      <c r="C5" s="46" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D5" s="47" t="s">
+      <c r="C5" s="49" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D5" s="50" t="s">
         <v>1015</v>
       </c>
-      <c r="E5" s="47" t="s">
-        <v>1097</v>
+      <c r="E5" s="50" t="s">
+        <v>1110</v>
       </c>
       <c r="F5" s="20"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="43" t="s">
-        <v>1098</v>
-      </c>
-      <c r="B6" s="45" t="s">
+      <c r="A6" s="46" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B6" s="48" t="s">
         <v>1011</v>
       </c>
-      <c r="C6" s="46" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D6" s="48" t="s">
+      <c r="C6" s="49" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D6" s="51" t="s">
         <v>1015</v>
       </c>
-      <c r="E6" s="48" t="s">
-        <v>1099</v>
-      </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="E6" s="51" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B7" s="45" t="s">
+      <c r="A7" s="46" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B7" s="48" t="s">
         <v>1022</v>
       </c>
-      <c r="C7" s="46" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D7" s="48" t="s">
+      <c r="C7" s="49" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D7" s="51" t="s">
         <v>1015</v>
       </c>
-      <c r="E7" s="48" t="s">
-        <v>1101</v>
-      </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
+      <c r="E7" s="51" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
       <c r="J7" s="20"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="43" t="s">
-        <v>1102</v>
-      </c>
-      <c r="B8" s="45" t="s">
+      <c r="A8" s="46" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B8" s="48" t="s">
         <v>1022</v>
       </c>
-      <c r="C8" s="46" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D8" s="48" t="s">
+      <c r="C8" s="49" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D8" s="51" t="s">
         <v>1015</v>
       </c>
-      <c r="E8" s="48" t="s">
-        <v>1103</v>
-      </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
+      <c r="E8" s="51" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
     </row>
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="43" t="s">
-        <v>1104</v>
-      </c>
-      <c r="B9" s="38" t="s">
+      <c r="A9" s="46" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>1022</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>1105</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>1106</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>1107</v>
+        <v>1118</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>1120</v>
       </c>
       <c r="F9" s="20"/>
-      <c r="G9" s="36"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="43" t="s">
-        <v>1108</v>
-      </c>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="46" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B10" s="48" t="s">
         <v>1011</v>
       </c>
-      <c r="C10" s="46" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48" t="s">
+      <c r="C10" s="49" t="s">
         <v>1109</v>
       </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="36"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="39"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="43" t="s">
-        <v>1110</v>
-      </c>
-      <c r="B11" s="45" t="s">
+      <c r="A11" s="46" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B11" s="48" t="s">
         <v>1011</v>
       </c>
-      <c r="C11" s="46" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48" t="s">
-        <v>1111</v>
-      </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="36"/>
+      <c r="C11" s="49" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F11" s="44"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="36"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="43" t="s">
-        <v>1112</v>
-      </c>
-      <c r="B12" s="38" t="s">
+      <c r="A12" s="46" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B12" s="41" t="s">
         <v>1022</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>1114</v>
-      </c>
-      <c r="E12" s="44" t="s">
-        <v>1115</v>
+      <c r="C12" s="40" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>1128</v>
       </c>
       <c r="F12" s="20"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="20"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="43" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B13" s="38" t="s">
+      <c r="A13" s="46" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B13" s="41" t="s">
         <v>1011</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E13" s="49" t="s">
-        <v>1119</v>
-      </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="C13" s="40" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="20"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="43" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B14" s="45" t="s">
+      <c r="A14" s="46" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B14" s="48" t="s">
         <v>1022</v>
       </c>
-      <c r="C14" s="46" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50" t="s">
-        <v>1121</v>
-      </c>
-      <c r="F14" s="36"/>
+      <c r="C14" s="49" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F14" s="39"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="43" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B15" s="38" t="s">
+      <c r="A15" s="46" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>1022</v>
       </c>
-      <c r="C15" s="37" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>1124</v>
+      <c r="C15" s="40" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>1137</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>1125</v>
-      </c>
-      <c r="F15" s="36"/>
+        <v>1138</v>
+      </c>
+      <c r="F15" s="39"/>
       <c r="G15" s="20"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="36"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="20"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="43" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B16" s="38" t="s">
+      <c r="A16" s="46" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B16" s="41" t="s">
         <v>1011</v>
       </c>
-      <c r="C16" s="37" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D16" s="52" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E16" s="52" t="s">
-        <v>1129</v>
-      </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="40" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D16" s="55" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="43" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B17" s="38" t="s">
+      <c r="A17" s="46" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B17" s="41" t="s">
         <v>1011</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="40" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D17" s="40" t="s">
         <v>1131</v>
       </c>
-      <c r="D17" s="37" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E17" s="49" t="s">
-        <v>1119</v>
-      </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="36"/>
+      <c r="E17" s="52" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="39"/>
       <c r="J17" s="20"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="43" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B18" s="45" t="s">
+      <c r="A18" s="46" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B18" s="48" t="s">
         <v>1011</v>
       </c>
-      <c r="C18" s="46" t="s">
-        <v>1096</v>
-      </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53" t="s">
-        <v>1133</v>
-      </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="49" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F18" s="44"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="20"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="43" t="s">
-        <v>1134</v>
-      </c>
-      <c r="B19" s="45" t="s">
+      <c r="A19" s="46" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B19" s="48" t="s">
         <v>1022</v>
       </c>
-      <c r="C19" s="46" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="47" t="s">
-        <v>1136</v>
-      </c>
-      <c r="F19" s="36"/>
+      <c r="C19" s="49" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="50" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F19" s="39"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="36"/>
+      <c r="I19" s="39"/>
       <c r="J19" s="20"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="43" t="s">
-        <v>1137</v>
-      </c>
-      <c r="B20" s="38" t="s">
+      <c r="A20" s="46" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B20" s="41" t="s">
         <v>1022</v>
       </c>
-      <c r="C20" s="37" t="s">
-        <v>1138</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>1139</v>
-      </c>
-      <c r="E20" s="44" t="s">
-        <v>1140</v>
-      </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
+      <c r="C20" s="40" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
       <c r="J20" s="20"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B21" s="32" t="s">
+      <c r="A21" s="45" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B21" s="35" t="s">
         <v>1011</v>
       </c>
-      <c r="C21" s="54" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>1143</v>
+      <c r="C21" s="57" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>1156</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" location="/CBS/nl/dataset/70739ned/table?dl=5A68C" display="&lt;CBS gemeentecode&gt;: code bestaande uit 6 karakters, zie https://opendata.cbs.nl/#/CBS/nl/dataset/70739ned/table?dl=5A68C of gebruik GM9001 voor Bonaire, GM9002 voor Sint Eustatius of GM9003 voor Saba.&#10;&#10;&lt;YYYYMMDD&gt;: datum van de verkiezing&#10;&#10;&lt;oplopend getal&gt;: getal tussen 000 en 999"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>